<commit_message>
2 Hour commit (Monday, 15:00)
</commit_message>
<xml_diff>
--- a/Dokumentation_0.3/Zeitplan.xlsx
+++ b/Dokumentation_0.3/Zeitplan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Moritz\Desktop\Projekte\probst-maveg\Dokumentation_0.3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AF43924-262B-4ACB-A33B-E0842724FDAC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9333BF78-ACB7-45D3-8CCF-72CEF90380F0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25180" windowHeight="16260" xr2:uid="{83867029-8E76-3D4F-AE7B-3038CD017D03}"/>
   </bookViews>
@@ -795,7 +795,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="137">
+  <cellXfs count="136">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -946,7 +946,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3173,8 +3172,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="12819579" y="3132941"/>
-          <a:ext cx="3438994" cy="2657104"/>
+          <a:off x="13117286" y="3057071"/>
+          <a:ext cx="3603930" cy="2576286"/>
           <a:chOff x="-199801" y="7333"/>
           <a:chExt cx="2044781" cy="1996547"/>
         </a:xfrm>
@@ -4927,6 +4926,74 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>99173</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>53541</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>88070</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>10051</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="70" name="Diamond 69">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2D463C77-AE13-4C05-A707-2ADFC2BFD148}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5882558" y="3726772"/>
+          <a:ext cx="164743" cy="147010"/>
+        </a:xfrm>
+        <a:prstGeom prst="diamond">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="tx1"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="de-CH" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -6146,8 +6213,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACB35978-8946-004E-AC9B-C0C1BFAB6460}">
   <dimension ref="A1:CL74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="AF29" sqref="AF29"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="L51" sqref="L51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -6165,13 +6232,13 @@
     <col min="82" max="82" width="2.58203125" customWidth="1"/>
     <col min="83" max="83" width="2.83203125" customWidth="1"/>
     <col min="84" max="84" width="3.4140625" customWidth="1"/>
-    <col min="85" max="85" width="3.4140625" style="69" customWidth="1"/>
+    <col min="85" max="85" width="3.4140625" style="68" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:90" x14ac:dyDescent="0.35">
       <c r="A1" s="18"/>
-      <c r="B1" s="62"/>
-      <c r="C1" s="62"/>
+      <c r="B1" s="61"/>
+      <c r="C1" s="61"/>
       <c r="D1" s="18"/>
       <c r="E1" s="18"/>
       <c r="F1" s="18"/>
@@ -6192,7 +6259,7 @@
       <c r="U1" s="18"/>
       <c r="V1" s="18"/>
       <c r="W1" s="18"/>
-      <c r="X1" s="63"/>
+      <c r="X1" s="62"/>
       <c r="Y1" s="18"/>
       <c r="Z1" s="18"/>
       <c r="AA1" s="18"/>
@@ -6253,7 +6320,7 @@
       <c r="CD1" s="18"/>
       <c r="CE1" s="18"/>
       <c r="CF1" s="18"/>
-      <c r="CG1" s="65"/>
+      <c r="CG1" s="64"/>
       <c r="CH1" s="18"/>
       <c r="CI1" s="18"/>
       <c r="CJ1" s="18"/>
@@ -6262,8 +6329,8 @@
     </row>
     <row r="2" spans="1:90" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="18"/>
-      <c r="B2" s="62"/>
-      <c r="C2" s="62"/>
+      <c r="B2" s="61"/>
+      <c r="C2" s="61"/>
       <c r="D2" s="18"/>
       <c r="E2" s="18"/>
       <c r="F2" s="18"/>
@@ -6284,7 +6351,7 @@
       <c r="U2" s="18"/>
       <c r="V2" s="18"/>
       <c r="W2" s="18"/>
-      <c r="X2" s="63"/>
+      <c r="X2" s="62"/>
       <c r="Y2" s="18"/>
       <c r="Z2" s="18"/>
       <c r="AA2" s="18"/>
@@ -6345,7 +6412,7 @@
       <c r="CD2" s="18"/>
       <c r="CE2" s="18"/>
       <c r="CF2" s="18"/>
-      <c r="CG2" s="65"/>
+      <c r="CG2" s="64"/>
       <c r="CH2" s="18"/>
       <c r="CI2" s="18"/>
       <c r="CJ2" s="18"/>
@@ -6353,229 +6420,229 @@
       <c r="CL2" s="18"/>
     </row>
     <row r="3" spans="1:90" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="115"/>
-      <c r="B3" s="118" t="s">
+      <c r="A3" s="114"/>
+      <c r="B3" s="117" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="103"/>
-      <c r="D3" s="119" t="s">
+      <c r="C3" s="102"/>
+      <c r="D3" s="118" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="119"/>
-      <c r="F3" s="119"/>
-      <c r="G3" s="103"/>
-      <c r="H3" s="118" t="s">
+      <c r="E3" s="118"/>
+      <c r="F3" s="118"/>
+      <c r="G3" s="102"/>
+      <c r="H3" s="117" t="s">
         <v>16</v>
       </c>
-      <c r="I3" s="119"/>
-      <c r="J3" s="119"/>
-      <c r="K3" s="119"/>
-      <c r="L3" s="119"/>
-      <c r="M3" s="119"/>
-      <c r="N3" s="119"/>
-      <c r="O3" s="103"/>
-      <c r="P3" s="118" t="s">
+      <c r="I3" s="118"/>
+      <c r="J3" s="118"/>
+      <c r="K3" s="118"/>
+      <c r="L3" s="118"/>
+      <c r="M3" s="118"/>
+      <c r="N3" s="118"/>
+      <c r="O3" s="102"/>
+      <c r="P3" s="117" t="s">
         <v>17</v>
       </c>
-      <c r="Q3" s="119"/>
-      <c r="R3" s="119"/>
-      <c r="S3" s="119"/>
-      <c r="T3" s="119"/>
-      <c r="U3" s="119"/>
-      <c r="V3" s="119"/>
-      <c r="W3" s="103"/>
-      <c r="X3" s="86"/>
-      <c r="Y3" s="118" t="s">
+      <c r="Q3" s="118"/>
+      <c r="R3" s="118"/>
+      <c r="S3" s="118"/>
+      <c r="T3" s="118"/>
+      <c r="U3" s="118"/>
+      <c r="V3" s="118"/>
+      <c r="W3" s="102"/>
+      <c r="X3" s="85"/>
+      <c r="Y3" s="117" t="s">
         <v>18</v>
       </c>
-      <c r="Z3" s="119"/>
-      <c r="AA3" s="119"/>
-      <c r="AB3" s="119"/>
-      <c r="AC3" s="119"/>
-      <c r="AD3" s="119"/>
-      <c r="AE3" s="119"/>
-      <c r="AF3" s="103"/>
-      <c r="AG3" s="119" t="s">
+      <c r="Z3" s="118"/>
+      <c r="AA3" s="118"/>
+      <c r="AB3" s="118"/>
+      <c r="AC3" s="118"/>
+      <c r="AD3" s="118"/>
+      <c r="AE3" s="118"/>
+      <c r="AF3" s="102"/>
+      <c r="AG3" s="118" t="s">
         <v>19</v>
       </c>
-      <c r="AH3" s="119"/>
-      <c r="AI3" s="119"/>
-      <c r="AJ3" s="119"/>
-      <c r="AK3" s="119"/>
-      <c r="AL3" s="119"/>
-      <c r="AM3" s="119"/>
-      <c r="AN3" s="103"/>
-      <c r="AO3" s="118" t="s">
+      <c r="AH3" s="118"/>
+      <c r="AI3" s="118"/>
+      <c r="AJ3" s="118"/>
+      <c r="AK3" s="118"/>
+      <c r="AL3" s="118"/>
+      <c r="AM3" s="118"/>
+      <c r="AN3" s="102"/>
+      <c r="AO3" s="117" t="s">
         <v>15</v>
       </c>
-      <c r="AP3" s="119"/>
-      <c r="AQ3" s="119"/>
-      <c r="AR3" s="119"/>
-      <c r="AS3" s="119"/>
-      <c r="AT3" s="119"/>
-      <c r="AU3" s="119"/>
-      <c r="AV3" s="103"/>
-      <c r="AW3" s="118" t="s">
+      <c r="AP3" s="118"/>
+      <c r="AQ3" s="118"/>
+      <c r="AR3" s="118"/>
+      <c r="AS3" s="118"/>
+      <c r="AT3" s="118"/>
+      <c r="AU3" s="118"/>
+      <c r="AV3" s="102"/>
+      <c r="AW3" s="117" t="s">
         <v>16</v>
       </c>
-      <c r="AX3" s="119"/>
-      <c r="AY3" s="119"/>
-      <c r="AZ3" s="119"/>
-      <c r="BA3" s="119"/>
-      <c r="BB3" s="119"/>
-      <c r="BC3" s="119"/>
-      <c r="BD3" s="103"/>
-      <c r="BE3" s="118" t="s">
+      <c r="AX3" s="118"/>
+      <c r="AY3" s="118"/>
+      <c r="AZ3" s="118"/>
+      <c r="BA3" s="118"/>
+      <c r="BB3" s="118"/>
+      <c r="BC3" s="118"/>
+      <c r="BD3" s="102"/>
+      <c r="BE3" s="117" t="s">
         <v>17</v>
       </c>
-      <c r="BF3" s="119"/>
-      <c r="BG3" s="119"/>
-      <c r="BH3" s="119"/>
-      <c r="BI3" s="119"/>
-      <c r="BJ3" s="119"/>
-      <c r="BK3" s="119"/>
-      <c r="BL3" s="103"/>
-      <c r="BM3" s="64"/>
-      <c r="BN3" s="118" t="s">
+      <c r="BF3" s="118"/>
+      <c r="BG3" s="118"/>
+      <c r="BH3" s="118"/>
+      <c r="BI3" s="118"/>
+      <c r="BJ3" s="118"/>
+      <c r="BK3" s="118"/>
+      <c r="BL3" s="102"/>
+      <c r="BM3" s="63"/>
+      <c r="BN3" s="117" t="s">
         <v>18</v>
       </c>
-      <c r="BO3" s="119"/>
-      <c r="BP3" s="119"/>
-      <c r="BQ3" s="119"/>
-      <c r="BR3" s="119"/>
-      <c r="BS3" s="119"/>
-      <c r="BT3" s="119"/>
-      <c r="BU3" s="119"/>
-      <c r="BV3" s="118" t="s">
+      <c r="BO3" s="118"/>
+      <c r="BP3" s="118"/>
+      <c r="BQ3" s="118"/>
+      <c r="BR3" s="118"/>
+      <c r="BS3" s="118"/>
+      <c r="BT3" s="118"/>
+      <c r="BU3" s="118"/>
+      <c r="BV3" s="117" t="s">
         <v>19</v>
       </c>
-      <c r="BW3" s="119"/>
-      <c r="BX3" s="119"/>
-      <c r="BY3" s="119"/>
-      <c r="BZ3" s="119"/>
-      <c r="CA3" s="119"/>
-      <c r="CB3" s="119"/>
-      <c r="CC3" s="119"/>
-      <c r="CD3" s="118" t="s">
+      <c r="BW3" s="118"/>
+      <c r="BX3" s="118"/>
+      <c r="BY3" s="118"/>
+      <c r="BZ3" s="118"/>
+      <c r="CA3" s="118"/>
+      <c r="CB3" s="118"/>
+      <c r="CC3" s="118"/>
+      <c r="CD3" s="117" t="s">
         <v>15</v>
       </c>
-      <c r="CE3" s="119"/>
-      <c r="CF3" s="119"/>
-      <c r="CG3" s="103"/>
+      <c r="CE3" s="118"/>
+      <c r="CF3" s="118"/>
+      <c r="CG3" s="102"/>
     </row>
     <row r="4" spans="1:90" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="116"/>
-      <c r="B4" s="111" t="s">
+      <c r="A4" s="115"/>
+      <c r="B4" s="110" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="112"/>
-      <c r="D4" s="113">
+      <c r="C4" s="111"/>
+      <c r="D4" s="112">
         <v>44293</v>
       </c>
-      <c r="E4" s="113"/>
-      <c r="F4" s="113"/>
-      <c r="G4" s="114"/>
-      <c r="H4" s="125">
+      <c r="E4" s="112"/>
+      <c r="F4" s="112"/>
+      <c r="G4" s="113"/>
+      <c r="H4" s="124">
         <v>44294</v>
       </c>
-      <c r="I4" s="126"/>
-      <c r="J4" s="126"/>
-      <c r="K4" s="126"/>
-      <c r="L4" s="126"/>
-      <c r="M4" s="126"/>
-      <c r="N4" s="126"/>
-      <c r="O4" s="127"/>
-      <c r="P4" s="125">
+      <c r="I4" s="125"/>
+      <c r="J4" s="125"/>
+      <c r="K4" s="125"/>
+      <c r="L4" s="125"/>
+      <c r="M4" s="125"/>
+      <c r="N4" s="125"/>
+      <c r="O4" s="126"/>
+      <c r="P4" s="124">
         <v>44295</v>
       </c>
-      <c r="Q4" s="126"/>
-      <c r="R4" s="126"/>
-      <c r="S4" s="126"/>
-      <c r="T4" s="126"/>
-      <c r="U4" s="126"/>
-      <c r="V4" s="126"/>
-      <c r="W4" s="127"/>
+      <c r="Q4" s="125"/>
+      <c r="R4" s="125"/>
+      <c r="S4" s="125"/>
+      <c r="T4" s="125"/>
+      <c r="U4" s="125"/>
+      <c r="V4" s="125"/>
+      <c r="W4" s="126"/>
       <c r="X4" s="46"/>
-      <c r="Y4" s="125">
+      <c r="Y4" s="124">
         <v>44298</v>
       </c>
-      <c r="Z4" s="126"/>
-      <c r="AA4" s="126"/>
-      <c r="AB4" s="126"/>
-      <c r="AC4" s="126"/>
-      <c r="AD4" s="126"/>
-      <c r="AE4" s="126"/>
-      <c r="AF4" s="127"/>
-      <c r="AG4" s="125">
+      <c r="Z4" s="125"/>
+      <c r="AA4" s="125"/>
+      <c r="AB4" s="125"/>
+      <c r="AC4" s="125"/>
+      <c r="AD4" s="125"/>
+      <c r="AE4" s="125"/>
+      <c r="AF4" s="126"/>
+      <c r="AG4" s="124">
         <v>44299</v>
       </c>
-      <c r="AH4" s="126"/>
-      <c r="AI4" s="126"/>
-      <c r="AJ4" s="126"/>
-      <c r="AK4" s="126"/>
-      <c r="AL4" s="126"/>
-      <c r="AM4" s="126"/>
-      <c r="AN4" s="127"/>
-      <c r="AO4" s="125">
+      <c r="AH4" s="125"/>
+      <c r="AI4" s="125"/>
+      <c r="AJ4" s="125"/>
+      <c r="AK4" s="125"/>
+      <c r="AL4" s="125"/>
+      <c r="AM4" s="125"/>
+      <c r="AN4" s="126"/>
+      <c r="AO4" s="124">
         <v>44300</v>
       </c>
-      <c r="AP4" s="126"/>
-      <c r="AQ4" s="126"/>
-      <c r="AR4" s="126"/>
-      <c r="AS4" s="126"/>
-      <c r="AT4" s="126"/>
-      <c r="AU4" s="126"/>
-      <c r="AV4" s="127"/>
-      <c r="AW4" s="125">
+      <c r="AP4" s="125"/>
+      <c r="AQ4" s="125"/>
+      <c r="AR4" s="125"/>
+      <c r="AS4" s="125"/>
+      <c r="AT4" s="125"/>
+      <c r="AU4" s="125"/>
+      <c r="AV4" s="126"/>
+      <c r="AW4" s="124">
         <v>44301</v>
       </c>
-      <c r="AX4" s="126"/>
-      <c r="AY4" s="126"/>
-      <c r="AZ4" s="126"/>
-      <c r="BA4" s="126"/>
-      <c r="BB4" s="126"/>
-      <c r="BC4" s="126"/>
-      <c r="BD4" s="127"/>
-      <c r="BE4" s="125">
+      <c r="AX4" s="125"/>
+      <c r="AY4" s="125"/>
+      <c r="AZ4" s="125"/>
+      <c r="BA4" s="125"/>
+      <c r="BB4" s="125"/>
+      <c r="BC4" s="125"/>
+      <c r="BD4" s="126"/>
+      <c r="BE4" s="124">
         <v>44302</v>
       </c>
-      <c r="BF4" s="126"/>
-      <c r="BG4" s="126"/>
-      <c r="BH4" s="126"/>
-      <c r="BI4" s="126"/>
-      <c r="BJ4" s="126"/>
-      <c r="BK4" s="126"/>
-      <c r="BL4" s="127"/>
+      <c r="BF4" s="125"/>
+      <c r="BG4" s="125"/>
+      <c r="BH4" s="125"/>
+      <c r="BI4" s="125"/>
+      <c r="BJ4" s="125"/>
+      <c r="BK4" s="125"/>
+      <c r="BL4" s="126"/>
       <c r="BM4" s="46"/>
-      <c r="BN4" s="125">
+      <c r="BN4" s="124">
         <v>44305</v>
       </c>
-      <c r="BO4" s="126"/>
-      <c r="BP4" s="126"/>
-      <c r="BQ4" s="126"/>
-      <c r="BR4" s="126"/>
-      <c r="BS4" s="126"/>
-      <c r="BT4" s="126"/>
-      <c r="BU4" s="127"/>
-      <c r="BV4" s="125">
+      <c r="BO4" s="125"/>
+      <c r="BP4" s="125"/>
+      <c r="BQ4" s="125"/>
+      <c r="BR4" s="125"/>
+      <c r="BS4" s="125"/>
+      <c r="BT4" s="125"/>
+      <c r="BU4" s="126"/>
+      <c r="BV4" s="124">
         <v>44306</v>
       </c>
-      <c r="BW4" s="126"/>
-      <c r="BX4" s="126"/>
-      <c r="BY4" s="126"/>
-      <c r="BZ4" s="126"/>
-      <c r="CA4" s="126"/>
-      <c r="CB4" s="126"/>
-      <c r="CC4" s="127"/>
-      <c r="CD4" s="125">
+      <c r="BW4" s="125"/>
+      <c r="BX4" s="125"/>
+      <c r="BY4" s="125"/>
+      <c r="BZ4" s="125"/>
+      <c r="CA4" s="125"/>
+      <c r="CB4" s="125"/>
+      <c r="CC4" s="126"/>
+      <c r="CD4" s="124">
         <v>44307</v>
       </c>
-      <c r="CE4" s="126"/>
-      <c r="CF4" s="126"/>
-      <c r="CG4" s="126"/>
+      <c r="CE4" s="125"/>
+      <c r="CF4" s="125"/>
+      <c r="CG4" s="125"/>
     </row>
     <row r="5" spans="1:90" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="117"/>
+      <c r="A5" s="116"/>
       <c r="B5" s="2" t="s">
         <v>2</v>
       </c>
@@ -6826,15 +6893,15 @@
       </c>
     </row>
     <row r="6" spans="1:90" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="120" t="s">
+      <c r="A6" s="119" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="121"/>
-      <c r="C6" s="121"/>
-      <c r="D6" s="121"/>
-      <c r="E6" s="121"/>
-      <c r="F6" s="121"/>
-      <c r="G6" s="122"/>
+      <c r="B6" s="120"/>
+      <c r="C6" s="120"/>
+      <c r="D6" s="120"/>
+      <c r="E6" s="120"/>
+      <c r="F6" s="120"/>
+      <c r="G6" s="121"/>
       <c r="H6" s="24"/>
       <c r="I6" s="24"/>
       <c r="J6" s="24"/>
@@ -6900,31 +6967,31 @@
       <c r="BR6" s="24"/>
       <c r="BS6" s="24"/>
       <c r="BT6" s="24"/>
-      <c r="BU6" s="74"/>
-      <c r="BV6" s="74"/>
+      <c r="BU6" s="73"/>
+      <c r="BV6" s="73"/>
       <c r="BW6" s="24"/>
       <c r="BX6" s="24"/>
       <c r="BY6" s="24"/>
       <c r="BZ6" s="24"/>
       <c r="CA6" s="24"/>
       <c r="CB6" s="24"/>
-      <c r="CC6" s="74"/>
-      <c r="CD6" s="74"/>
+      <c r="CC6" s="73"/>
+      <c r="CD6" s="73"/>
       <c r="CE6" s="43"/>
       <c r="CF6" s="43"/>
       <c r="CG6" s="44"/>
     </row>
     <row r="7" spans="1:90" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="123" t="s">
+      <c r="A7" s="122" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="99">
+      <c r="B7" s="98">
         <v>1</v>
       </c>
-      <c r="C7" s="105">
+      <c r="C7" s="104">
         <v>1</v>
       </c>
-      <c r="D7" s="70"/>
+      <c r="D7" s="69"/>
       <c r="E7" s="10"/>
       <c r="F7" s="10"/>
       <c r="G7" s="11"/>
@@ -7005,13 +7072,13 @@
       <c r="CD7" s="12"/>
       <c r="CE7" s="13"/>
       <c r="CF7" s="13"/>
-      <c r="CG7" s="66"/>
+      <c r="CG7" s="65"/>
     </row>
     <row r="8" spans="1:90" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="124"/>
-      <c r="B8" s="100"/>
-      <c r="C8" s="106"/>
-      <c r="D8" s="83"/>
+      <c r="A8" s="123"/>
+      <c r="B8" s="99"/>
+      <c r="C8" s="105"/>
+      <c r="D8" s="82"/>
       <c r="E8" s="54"/>
       <c r="F8" s="6"/>
       <c r="G8" s="16"/>
@@ -7095,18 +7162,18 @@
       <c r="CG8" s="3"/>
     </row>
     <row r="9" spans="1:90" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="107" t="s">
+      <c r="A9" s="106" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="109">
+      <c r="B9" s="108">
         <v>2</v>
       </c>
-      <c r="C9" s="110">
+      <c r="C9" s="109">
         <v>1</v>
       </c>
       <c r="D9" s="20"/>
-      <c r="E9" s="71"/>
-      <c r="F9" s="71"/>
+      <c r="E9" s="70"/>
+      <c r="F9" s="70"/>
       <c r="G9" s="21"/>
       <c r="H9" s="19"/>
       <c r="I9" s="20"/>
@@ -7185,17 +7252,17 @@
       <c r="CD9" s="12"/>
       <c r="CE9" s="13"/>
       <c r="CF9" s="13"/>
-      <c r="CG9" s="66"/>
+      <c r="CG9" s="65"/>
     </row>
     <row r="10" spans="1:90" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="108"/>
-      <c r="B10" s="100"/>
-      <c r="C10" s="106"/>
+      <c r="A10" s="107"/>
+      <c r="B10" s="99"/>
+      <c r="C10" s="105"/>
       <c r="D10" s="6"/>
-      <c r="E10" s="83"/>
+      <c r="E10" s="82"/>
       <c r="F10" s="6"/>
       <c r="G10" s="6"/>
-      <c r="H10" s="85"/>
+      <c r="H10" s="84"/>
       <c r="I10" s="6"/>
       <c r="J10" s="6"/>
       <c r="K10" s="6"/>
@@ -7275,20 +7342,20 @@
       <c r="CG10" s="3"/>
     </row>
     <row r="11" spans="1:90" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="107" t="s">
+      <c r="A11" s="106" t="s">
         <v>45</v>
       </c>
-      <c r="B11" s="109">
+      <c r="B11" s="108">
         <v>2</v>
       </c>
-      <c r="C11" s="110">
+      <c r="C11" s="109">
         <v>4</v>
       </c>
       <c r="D11" s="19"/>
       <c r="E11" s="20"/>
       <c r="F11" s="20"/>
-      <c r="G11" s="71"/>
-      <c r="H11" s="71"/>
+      <c r="G11" s="70"/>
+      <c r="H11" s="70"/>
       <c r="I11" s="20"/>
       <c r="J11" s="20"/>
       <c r="K11" s="20"/>
@@ -7365,18 +7432,18 @@
       <c r="CD11" s="12"/>
       <c r="CE11" s="13"/>
       <c r="CF11" s="13"/>
-      <c r="CG11" s="66"/>
+      <c r="CG11" s="65"/>
     </row>
     <row r="12" spans="1:90" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="108"/>
-      <c r="B12" s="100"/>
-      <c r="C12" s="106"/>
+      <c r="A12" s="107"/>
+      <c r="B12" s="99"/>
+      <c r="C12" s="105"/>
       <c r="D12" s="2"/>
       <c r="E12" s="6"/>
-      <c r="F12" s="83"/>
-      <c r="G12" s="84"/>
-      <c r="H12" s="83"/>
-      <c r="I12" s="83"/>
+      <c r="F12" s="82"/>
+      <c r="G12" s="83"/>
+      <c r="H12" s="82"/>
+      <c r="I12" s="82"/>
       <c r="J12" s="6"/>
       <c r="K12" s="6"/>
       <c r="L12" s="6"/>
@@ -7455,13 +7522,13 @@
       <c r="CG12" s="3"/>
     </row>
     <row r="13" spans="1:90" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="107" t="s">
+      <c r="A13" s="106" t="s">
         <v>46</v>
       </c>
-      <c r="B13" s="109">
+      <c r="B13" s="108">
         <v>2</v>
       </c>
-      <c r="C13" s="110">
+      <c r="C13" s="109">
         <v>2</v>
       </c>
       <c r="D13" s="19"/>
@@ -7469,8 +7536,8 @@
       <c r="F13" s="20"/>
       <c r="G13" s="11"/>
       <c r="H13" s="19"/>
-      <c r="I13" s="71"/>
-      <c r="J13" s="87"/>
+      <c r="I13" s="70"/>
+      <c r="J13" s="86"/>
       <c r="K13" s="20"/>
       <c r="L13" s="20"/>
       <c r="M13" s="20"/>
@@ -7545,20 +7612,20 @@
       <c r="CD13" s="12"/>
       <c r="CE13" s="13"/>
       <c r="CF13" s="13"/>
-      <c r="CG13" s="66"/>
+      <c r="CG13" s="65"/>
     </row>
     <row r="14" spans="1:90" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="108"/>
-      <c r="B14" s="100"/>
-      <c r="C14" s="106"/>
+      <c r="A14" s="107"/>
+      <c r="B14" s="99"/>
+      <c r="C14" s="105"/>
       <c r="D14" s="2"/>
       <c r="E14" s="6"/>
       <c r="F14" s="6"/>
       <c r="G14" s="6"/>
       <c r="H14" s="2"/>
       <c r="I14" s="6"/>
-      <c r="J14" s="83"/>
-      <c r="K14" s="83"/>
+      <c r="J14" s="82"/>
+      <c r="K14" s="82"/>
       <c r="L14" s="6"/>
       <c r="M14" s="6"/>
       <c r="N14" s="6"/>
@@ -7635,13 +7702,13 @@
       <c r="CG14" s="3"/>
     </row>
     <row r="15" spans="1:90" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="107" t="s">
+      <c r="A15" s="106" t="s">
         <v>47</v>
       </c>
-      <c r="B15" s="109">
+      <c r="B15" s="108">
         <v>2</v>
       </c>
-      <c r="C15" s="110">
+      <c r="C15" s="109">
         <v>1</v>
       </c>
       <c r="D15" s="20"/>
@@ -7651,8 +7718,8 @@
       <c r="H15" s="19"/>
       <c r="I15" s="20"/>
       <c r="J15" s="55"/>
-      <c r="K15" s="71"/>
-      <c r="L15" s="87"/>
+      <c r="K15" s="70"/>
+      <c r="L15" s="86"/>
       <c r="M15" s="20"/>
       <c r="N15" s="20"/>
       <c r="O15" s="21"/>
@@ -7725,12 +7792,12 @@
       <c r="CD15" s="12"/>
       <c r="CE15" s="13"/>
       <c r="CF15" s="13"/>
-      <c r="CG15" s="66"/>
+      <c r="CG15" s="65"/>
     </row>
     <row r="16" spans="1:90" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="108"/>
-      <c r="B16" s="100"/>
-      <c r="C16" s="106"/>
+      <c r="A16" s="107"/>
+      <c r="B16" s="99"/>
+      <c r="C16" s="105"/>
       <c r="D16" s="6"/>
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
@@ -7739,11 +7806,11 @@
       <c r="I16" s="6"/>
       <c r="J16" s="6"/>
       <c r="K16" s="6"/>
-      <c r="L16" s="83"/>
+      <c r="L16" s="82"/>
       <c r="M16" s="54"/>
       <c r="N16" s="6"/>
       <c r="O16" s="56"/>
-      <c r="P16" s="85"/>
+      <c r="P16" s="84"/>
       <c r="Q16" s="54"/>
       <c r="R16" s="54"/>
       <c r="S16" s="54"/>
@@ -7815,13 +7882,13 @@
       <c r="CG16" s="3"/>
     </row>
     <row r="17" spans="1:85" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="130" t="s">
+      <c r="A17" s="129" t="s">
         <v>7</v>
       </c>
-      <c r="B17" s="99">
+      <c r="B17" s="98">
         <v>2</v>
       </c>
-      <c r="C17" s="105">
+      <c r="C17" s="104">
         <v>1</v>
       </c>
       <c r="D17" s="10"/>
@@ -7833,8 +7900,8 @@
       <c r="J17" s="10"/>
       <c r="K17" s="10"/>
       <c r="L17" s="58"/>
-      <c r="M17" s="70"/>
-      <c r="N17" s="87"/>
+      <c r="M17" s="69"/>
+      <c r="N17" s="86"/>
       <c r="O17" s="11"/>
       <c r="P17" s="9"/>
       <c r="Q17" s="10"/>
@@ -7905,12 +7972,12 @@
       <c r="CD17" s="12"/>
       <c r="CE17" s="13"/>
       <c r="CF17" s="13"/>
-      <c r="CG17" s="66"/>
+      <c r="CG17" s="65"/>
     </row>
     <row r="18" spans="1:85" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A18" s="108"/>
-      <c r="B18" s="100"/>
-      <c r="C18" s="106"/>
+      <c r="A18" s="107"/>
+      <c r="B18" s="99"/>
+      <c r="C18" s="105"/>
       <c r="D18" s="6"/>
       <c r="E18" s="6"/>
       <c r="F18" s="6"/>
@@ -7920,7 +7987,7 @@
       <c r="J18" s="6"/>
       <c r="K18" s="6"/>
       <c r="L18" s="6"/>
-      <c r="M18" s="83"/>
+      <c r="M18" s="82"/>
       <c r="N18" s="6"/>
       <c r="O18" s="16"/>
       <c r="P18" s="2"/>
@@ -7995,14 +8062,14 @@
       <c r="CG18" s="3"/>
     </row>
     <row r="19" spans="1:85" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="128" t="s">
+      <c r="A19" s="127" t="s">
         <v>48</v>
       </c>
-      <c r="B19" s="99">
+      <c r="B19" s="98">
         <v>1</v>
       </c>
-      <c r="C19" s="105">
-        <v>1</v>
+      <c r="C19" s="104">
+        <v>3</v>
       </c>
       <c r="D19" s="10"/>
       <c r="E19" s="10"/>
@@ -8015,7 +8082,7 @@
       <c r="L19" s="10"/>
       <c r="M19" s="10"/>
       <c r="N19" s="59"/>
-      <c r="O19" s="72"/>
+      <c r="O19" s="71"/>
       <c r="P19" s="9"/>
       <c r="Q19" s="10"/>
       <c r="R19" s="10"/>
@@ -8085,12 +8152,12 @@
       <c r="CD19" s="12"/>
       <c r="CE19" s="13"/>
       <c r="CF19" s="13"/>
-      <c r="CG19" s="66"/>
+      <c r="CG19" s="65"/>
     </row>
     <row r="20" spans="1:85" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="129"/>
-      <c r="B20" s="100"/>
-      <c r="C20" s="106"/>
+      <c r="A20" s="128"/>
+      <c r="B20" s="99"/>
+      <c r="C20" s="105"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
@@ -8101,9 +8168,9 @@
       <c r="K20" s="6"/>
       <c r="L20" s="6"/>
       <c r="M20" s="6"/>
-      <c r="N20" s="83"/>
-      <c r="O20" s="84"/>
-      <c r="P20" s="2"/>
+      <c r="N20" s="82"/>
+      <c r="O20" s="83"/>
+      <c r="P20" s="135"/>
       <c r="Q20" s="6"/>
       <c r="R20" s="6"/>
       <c r="S20" s="6"/>
@@ -8175,15 +8242,15 @@
       <c r="CG20" s="3"/>
     </row>
     <row r="21" spans="1:85" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="131" t="s">
+      <c r="A21" s="130" t="s">
         <v>20</v>
       </c>
-      <c r="B21" s="132"/>
-      <c r="C21" s="132"/>
-      <c r="D21" s="132"/>
-      <c r="E21" s="132"/>
-      <c r="F21" s="132"/>
-      <c r="G21" s="133"/>
+      <c r="B21" s="131"/>
+      <c r="C21" s="131"/>
+      <c r="D21" s="131"/>
+      <c r="E21" s="131"/>
+      <c r="F21" s="131"/>
+      <c r="G21" s="132"/>
       <c r="H21" s="27"/>
       <c r="I21" s="27"/>
       <c r="J21" s="27"/>
@@ -8264,13 +8331,15 @@
       <c r="CG21" s="44"/>
     </row>
     <row r="22" spans="1:85" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="130" t="s">
+      <c r="A22" s="129" t="s">
         <v>49</v>
       </c>
-      <c r="B22" s="99">
+      <c r="B22" s="98">
         <v>1</v>
       </c>
-      <c r="C22" s="105"/>
+      <c r="C22" s="104">
+        <v>1</v>
+      </c>
       <c r="D22" s="10"/>
       <c r="E22" s="10"/>
       <c r="F22" s="10"/>
@@ -8279,11 +8348,11 @@
       <c r="I22" s="10"/>
       <c r="J22" s="10"/>
       <c r="K22" s="10"/>
-      <c r="L22" s="58"/>
-      <c r="M22" s="58"/>
+      <c r="L22" s="10"/>
+      <c r="M22" s="10"/>
       <c r="N22" s="10"/>
       <c r="O22" s="11"/>
-      <c r="Q22" s="73"/>
+      <c r="Q22" s="72"/>
       <c r="R22" s="10"/>
       <c r="S22" s="10"/>
       <c r="T22" s="10"/>
@@ -8351,12 +8420,12 @@
       <c r="CD22" s="12"/>
       <c r="CE22" s="13"/>
       <c r="CF22" s="13"/>
-      <c r="CG22" s="66"/>
+      <c r="CG22" s="65"/>
     </row>
     <row r="23" spans="1:85" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="108"/>
-      <c r="B23" s="100"/>
-      <c r="C23" s="106"/>
+      <c r="A23" s="107"/>
+      <c r="B23" s="99"/>
+      <c r="C23" s="105"/>
       <c r="D23" s="6"/>
       <c r="E23" s="6"/>
       <c r="F23" s="6"/>
@@ -8371,8 +8440,7 @@
       <c r="O23" s="16"/>
       <c r="P23" s="2"/>
       <c r="Q23" s="6"/>
-      <c r="R23" s="83"/>
-      <c r="S23" s="6"/>
+      <c r="S23" s="82"/>
       <c r="T23" s="6"/>
       <c r="U23" s="6"/>
       <c r="V23" s="6"/>
@@ -8441,13 +8509,15 @@
       <c r="CG23" s="3"/>
     </row>
     <row r="24" spans="1:85" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="123" t="s">
+      <c r="A24" s="122" t="s">
         <v>50</v>
       </c>
-      <c r="B24" s="99">
+      <c r="B24" s="98">
         <v>2</v>
       </c>
-      <c r="C24" s="105"/>
+      <c r="C24" s="104">
+        <v>2</v>
+      </c>
       <c r="D24" s="10"/>
       <c r="E24" s="10"/>
       <c r="F24" s="10"/>
@@ -8457,12 +8527,12 @@
       <c r="J24" s="10"/>
       <c r="K24" s="10"/>
       <c r="L24" s="10"/>
-      <c r="M24" s="58"/>
-      <c r="N24" s="58"/>
+      <c r="M24" s="10"/>
+      <c r="N24" s="10"/>
       <c r="O24" s="11"/>
       <c r="Q24" s="58"/>
-      <c r="R24" s="70"/>
-      <c r="S24" s="70"/>
+      <c r="R24" s="69"/>
+      <c r="S24" s="69"/>
       <c r="T24" s="10"/>
       <c r="U24" s="10"/>
       <c r="V24" s="10"/>
@@ -8528,12 +8598,12 @@
       <c r="CD24" s="12"/>
       <c r="CE24" s="13"/>
       <c r="CF24" s="13"/>
-      <c r="CG24" s="66"/>
+      <c r="CG24" s="65"/>
     </row>
     <row r="25" spans="1:85" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A25" s="108"/>
-      <c r="B25" s="100"/>
-      <c r="C25" s="106"/>
+      <c r="A25" s="107"/>
+      <c r="B25" s="99"/>
+      <c r="C25" s="105"/>
       <c r="D25" s="6"/>
       <c r="E25" s="6"/>
       <c r="F25" s="6"/>
@@ -8549,9 +8619,8 @@
       <c r="P25" s="2"/>
       <c r="Q25" s="6"/>
       <c r="R25" s="6"/>
-      <c r="S25" s="83"/>
-      <c r="T25" s="83"/>
-      <c r="U25" s="6"/>
+      <c r="T25" s="82"/>
+      <c r="U25" s="82"/>
       <c r="V25" s="6"/>
       <c r="W25" s="16"/>
       <c r="X25" s="46"/>
@@ -8618,13 +8687,15 @@
       <c r="CG25" s="3"/>
     </row>
     <row r="26" spans="1:85" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="130" t="s">
+      <c r="A26" s="129" t="s">
         <v>51</v>
       </c>
-      <c r="B26" s="99">
+      <c r="B26" s="98">
         <v>2</v>
       </c>
-      <c r="C26" s="105"/>
+      <c r="C26" s="104">
+        <v>2</v>
+      </c>
       <c r="D26" s="10"/>
       <c r="E26" s="10"/>
       <c r="F26" s="10"/>
@@ -8636,11 +8707,13 @@
       <c r="L26" s="10"/>
       <c r="M26" s="10"/>
       <c r="N26" s="10"/>
-      <c r="O26" s="59"/>
-      <c r="P26" s="57"/>
+      <c r="O26" s="11"/>
+      <c r="P26" s="10"/>
       <c r="Q26" s="10"/>
-      <c r="T26" s="70"/>
-      <c r="U26" s="70"/>
+      <c r="R26" s="10"/>
+      <c r="S26" s="10"/>
+      <c r="T26" s="69"/>
+      <c r="U26" s="69"/>
       <c r="V26" s="10"/>
       <c r="W26" s="11"/>
       <c r="X26" s="46"/>
@@ -8704,12 +8777,12 @@
       <c r="CD26" s="12"/>
       <c r="CE26" s="13"/>
       <c r="CF26" s="13"/>
-      <c r="CG26" s="66"/>
+      <c r="CG26" s="65"/>
     </row>
     <row r="27" spans="1:85" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A27" s="108"/>
-      <c r="B27" s="100"/>
-      <c r="C27" s="106"/>
+      <c r="A27" s="107"/>
+      <c r="B27" s="99"/>
+      <c r="C27" s="105"/>
       <c r="D27" s="6"/>
       <c r="E27" s="6"/>
       <c r="F27" s="6"/>
@@ -8727,9 +8800,8 @@
       <c r="R27" s="6"/>
       <c r="S27" s="6"/>
       <c r="T27" s="6"/>
-      <c r="U27" s="83"/>
-      <c r="V27" s="83"/>
-      <c r="W27" s="16"/>
+      <c r="V27" s="82"/>
+      <c r="W27" s="82"/>
       <c r="X27" s="46"/>
       <c r="Y27" s="2"/>
       <c r="Z27" s="6"/>
@@ -8797,10 +8869,12 @@
       <c r="A28" s="40" t="s">
         <v>52</v>
       </c>
-      <c r="B28" s="99">
+      <c r="B28" s="98">
         <v>1</v>
       </c>
-      <c r="C28" s="105"/>
+      <c r="C28" s="104">
+        <v>1</v>
+      </c>
       <c r="D28" s="10"/>
       <c r="E28" s="10"/>
       <c r="F28" s="10"/>
@@ -8817,7 +8891,7 @@
       <c r="Q28" s="58"/>
       <c r="R28" s="10"/>
       <c r="S28" s="10"/>
-      <c r="V28" s="70"/>
+      <c r="V28" s="69"/>
       <c r="W28" s="11"/>
       <c r="X28" s="46"/>
       <c r="Y28" s="9"/>
@@ -8880,12 +8954,12 @@
       <c r="CD28" s="12"/>
       <c r="CE28" s="13"/>
       <c r="CF28" s="13"/>
-      <c r="CG28" s="66"/>
+      <c r="CG28" s="65"/>
     </row>
     <row r="29" spans="1:85" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A29" s="41"/>
-      <c r="B29" s="100"/>
-      <c r="C29" s="106"/>
+      <c r="B29" s="99"/>
+      <c r="C29" s="105"/>
       <c r="D29" s="6"/>
       <c r="E29" s="6"/>
       <c r="F29" s="6"/>
@@ -8905,9 +8979,8 @@
       <c r="T29" s="6"/>
       <c r="U29" s="6"/>
       <c r="V29" s="6"/>
-      <c r="W29" s="84"/>
       <c r="X29" s="46"/>
-      <c r="Y29" s="2"/>
+      <c r="Y29" s="83"/>
       <c r="Z29" s="6"/>
       <c r="AA29" s="6"/>
       <c r="AB29" s="6"/>
@@ -8973,10 +9046,10 @@
       <c r="A30" s="40" t="s">
         <v>53</v>
       </c>
-      <c r="B30" s="99">
+      <c r="B30" s="98">
         <v>3</v>
       </c>
-      <c r="C30" s="105"/>
+      <c r="C30" s="104"/>
       <c r="D30" s="10"/>
       <c r="E30" s="10"/>
       <c r="F30" s="10"/>
@@ -8993,11 +9066,12 @@
       <c r="R30" s="10"/>
       <c r="S30" s="10"/>
       <c r="T30" s="10"/>
-      <c r="U30" s="58"/>
-      <c r="W30" s="70"/>
+      <c r="U30" s="10"/>
+      <c r="V30" s="10"/>
+      <c r="W30" s="69"/>
       <c r="X30" s="46"/>
-      <c r="Y30" s="87"/>
-      <c r="Z30" s="70"/>
+      <c r="Y30" s="86"/>
+      <c r="Z30" s="69"/>
       <c r="AA30" s="10"/>
       <c r="AB30" s="10"/>
       <c r="AC30" s="10"/>
@@ -9056,12 +9130,12 @@
       <c r="CD30" s="12"/>
       <c r="CE30" s="13"/>
       <c r="CF30" s="13"/>
-      <c r="CG30" s="66"/>
+      <c r="CG30" s="65"/>
     </row>
     <row r="31" spans="1:85" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A31" s="41"/>
-      <c r="B31" s="100"/>
-      <c r="C31" s="106"/>
+      <c r="B31" s="99"/>
+      <c r="C31" s="105"/>
       <c r="D31" s="6"/>
       <c r="E31" s="6"/>
       <c r="F31" s="6"/>
@@ -9083,7 +9157,7 @@
       <c r="V31" s="54"/>
       <c r="W31" s="56"/>
       <c r="X31" s="46"/>
-      <c r="Y31" s="85"/>
+      <c r="Y31" s="84"/>
       <c r="Z31" s="54"/>
       <c r="AA31" s="54"/>
       <c r="AB31" s="6"/>
@@ -9149,10 +9223,10 @@
       <c r="A32" s="40" t="s">
         <v>54</v>
       </c>
-      <c r="B32" s="99">
+      <c r="B32" s="98">
         <v>2</v>
       </c>
-      <c r="C32" s="105"/>
+      <c r="C32" s="104"/>
       <c r="D32" s="10"/>
       <c r="E32" s="10"/>
       <c r="F32" s="10"/>
@@ -9173,8 +9247,8 @@
       <c r="V32" s="10"/>
       <c r="W32" s="10"/>
       <c r="X32" s="46"/>
-      <c r="AA32" s="70"/>
-      <c r="AB32" s="70"/>
+      <c r="AA32" s="69"/>
+      <c r="AB32" s="69"/>
       <c r="AC32" s="10"/>
       <c r="AD32" s="10"/>
       <c r="AE32" s="10"/>
@@ -9231,12 +9305,12 @@
       <c r="CD32" s="12"/>
       <c r="CE32" s="13"/>
       <c r="CF32" s="13"/>
-      <c r="CG32" s="66"/>
+      <c r="CG32" s="65"/>
     </row>
     <row r="33" spans="1:85" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A33" s="41"/>
-      <c r="B33" s="100"/>
-      <c r="C33" s="106"/>
+      <c r="B33" s="99"/>
+      <c r="C33" s="105"/>
       <c r="D33" s="6"/>
       <c r="E33" s="6"/>
       <c r="F33" s="6"/>
@@ -9324,10 +9398,10 @@
       <c r="A34" s="52" t="s">
         <v>14</v>
       </c>
-      <c r="B34" s="99">
+      <c r="B34" s="98">
         <v>4</v>
       </c>
-      <c r="C34" s="105"/>
+      <c r="C34" s="104"/>
       <c r="D34" s="10"/>
       <c r="E34" s="10"/>
       <c r="F34" s="10"/>
@@ -9343,18 +9417,17 @@
       <c r="P34" s="9"/>
       <c r="Q34" s="10"/>
       <c r="R34" s="10"/>
-      <c r="S34" s="58"/>
-      <c r="T34" s="58"/>
-      <c r="U34" s="18"/>
-      <c r="V34" s="18"/>
-      <c r="W34" s="60"/>
+      <c r="T34" s="10"/>
+      <c r="U34" s="10"/>
+      <c r="V34" s="10"/>
+      <c r="W34" s="10"/>
       <c r="X34" s="46"/>
       <c r="Y34" s="19"/>
       <c r="Z34" s="20"/>
-      <c r="AD34" s="71"/>
-      <c r="AE34" s="71"/>
-      <c r="AF34" s="71"/>
-      <c r="AG34" s="71"/>
+      <c r="AD34" s="70"/>
+      <c r="AE34" s="70"/>
+      <c r="AF34" s="70"/>
+      <c r="AG34" s="70"/>
       <c r="AH34" s="10"/>
       <c r="AI34" s="10"/>
       <c r="AJ34" s="10"/>
@@ -9406,12 +9479,12 @@
       <c r="CD34" s="12"/>
       <c r="CE34" s="13"/>
       <c r="CF34" s="13"/>
-      <c r="CG34" s="66"/>
+      <c r="CG34" s="65"/>
     </row>
     <row r="35" spans="1:85" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A35" s="53"/>
-      <c r="B35" s="100"/>
-      <c r="C35" s="106"/>
+      <c r="B35" s="99"/>
+      <c r="C35" s="105"/>
       <c r="D35" s="6"/>
       <c r="E35" s="6"/>
       <c r="F35" s="6"/>
@@ -9499,10 +9572,10 @@
       <c r="A36" s="40" t="s">
         <v>55</v>
       </c>
-      <c r="B36" s="99">
+      <c r="B36" s="98">
         <v>2</v>
       </c>
-      <c r="C36" s="105"/>
+      <c r="C36" s="104"/>
       <c r="D36" s="10"/>
       <c r="E36" s="10"/>
       <c r="F36" s="10"/>
@@ -9530,8 +9603,8 @@
       <c r="AC36" s="10"/>
       <c r="AD36" s="10"/>
       <c r="AE36" s="58"/>
-      <c r="AH36" s="71"/>
-      <c r="AI36" s="71"/>
+      <c r="AH36" s="70"/>
+      <c r="AI36" s="70"/>
       <c r="AJ36" s="10"/>
       <c r="AK36" s="10"/>
       <c r="AL36" s="10"/>
@@ -9581,12 +9654,12 @@
       <c r="CD36" s="12"/>
       <c r="CE36" s="13"/>
       <c r="CF36" s="13"/>
-      <c r="CG36" s="66"/>
+      <c r="CG36" s="65"/>
     </row>
     <row r="37" spans="1:85" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A37" s="41"/>
-      <c r="B37" s="100"/>
-      <c r="C37" s="106"/>
+      <c r="B37" s="99"/>
+      <c r="C37" s="105"/>
       <c r="D37" s="6"/>
       <c r="E37" s="6"/>
       <c r="F37" s="6"/>
@@ -9674,10 +9747,10 @@
       <c r="A38" s="40" t="s">
         <v>56</v>
       </c>
-      <c r="B38" s="99">
+      <c r="B38" s="98">
         <v>2</v>
       </c>
-      <c r="C38" s="105"/>
+      <c r="C38" s="104"/>
       <c r="D38" s="10"/>
       <c r="E38" s="10"/>
       <c r="F38" s="10"/>
@@ -9705,8 +9778,8 @@
       <c r="AB38" s="10"/>
       <c r="AC38" s="10"/>
       <c r="AF38" s="59"/>
-      <c r="AJ38" s="70"/>
-      <c r="AK38" s="70"/>
+      <c r="AJ38" s="69"/>
+      <c r="AK38" s="69"/>
       <c r="AL38" s="10"/>
       <c r="AM38" s="10"/>
       <c r="AN38" s="11"/>
@@ -9754,12 +9827,12 @@
       <c r="CD38" s="12"/>
       <c r="CE38" s="13"/>
       <c r="CF38" s="13"/>
-      <c r="CG38" s="66"/>
+      <c r="CG38" s="65"/>
     </row>
     <row r="39" spans="1:85" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A39" s="41"/>
-      <c r="B39" s="100"/>
-      <c r="C39" s="106"/>
+      <c r="B39" s="99"/>
+      <c r="C39" s="105"/>
       <c r="D39" s="6"/>
       <c r="E39" s="6"/>
       <c r="F39" s="6"/>
@@ -9936,10 +10009,10 @@
       <c r="A41" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="B41" s="99">
+      <c r="B41" s="98">
         <v>2</v>
       </c>
-      <c r="C41" s="105"/>
+      <c r="C41" s="104"/>
       <c r="D41" s="10"/>
       <c r="E41" s="10"/>
       <c r="F41" s="10"/>
@@ -9972,8 +10045,8 @@
       <c r="AG41" s="10"/>
       <c r="AI41" s="10"/>
       <c r="AJ41" s="10"/>
-      <c r="AN41" s="70"/>
-      <c r="AO41" s="70"/>
+      <c r="AN41" s="69"/>
+      <c r="AO41" s="69"/>
       <c r="AP41" s="10"/>
       <c r="AQ41" s="10"/>
       <c r="AR41" s="10"/>
@@ -10017,12 +10090,12 @@
       <c r="CD41" s="9"/>
       <c r="CE41" s="10"/>
       <c r="CF41" s="10"/>
-      <c r="CG41" s="67"/>
+      <c r="CG41" s="66"/>
     </row>
     <row r="42" spans="1:85" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A42" s="41"/>
-      <c r="B42" s="100"/>
-      <c r="C42" s="106"/>
+      <c r="B42" s="99"/>
+      <c r="C42" s="105"/>
       <c r="D42" s="6"/>
       <c r="E42" s="6"/>
       <c r="F42" s="6"/>
@@ -10110,10 +10183,10 @@
       <c r="A43" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="B43" s="99">
+      <c r="B43" s="98">
         <v>2</v>
       </c>
-      <c r="C43" s="105"/>
+      <c r="C43" s="104"/>
       <c r="D43" s="10"/>
       <c r="E43" s="10"/>
       <c r="F43" s="10"/>
@@ -10148,8 +10221,8 @@
       <c r="AI43" s="10"/>
       <c r="AJ43" s="10"/>
       <c r="AM43" s="58"/>
-      <c r="AP43" s="70"/>
-      <c r="AQ43" s="70"/>
+      <c r="AP43" s="69"/>
+      <c r="AQ43" s="69"/>
       <c r="AR43" s="10"/>
       <c r="AS43" s="10"/>
       <c r="AT43" s="10"/>
@@ -10191,12 +10264,12 @@
       <c r="CD43" s="9"/>
       <c r="CE43" s="10"/>
       <c r="CF43" s="10"/>
-      <c r="CG43" s="67"/>
+      <c r="CG43" s="66"/>
     </row>
     <row r="44" spans="1:85" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A44" s="41"/>
-      <c r="B44" s="100"/>
-      <c r="C44" s="106"/>
+      <c r="B44" s="99"/>
+      <c r="C44" s="105"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
@@ -10284,10 +10357,10 @@
       <c r="A45" s="40" t="s">
         <v>34</v>
       </c>
-      <c r="B45" s="99">
+      <c r="B45" s="98">
         <v>4</v>
       </c>
-      <c r="C45" s="105"/>
+      <c r="C45" s="104"/>
       <c r="D45" s="10"/>
       <c r="E45" s="10"/>
       <c r="F45" s="10"/>
@@ -10325,10 +10398,10 @@
       <c r="AL45" s="10"/>
       <c r="AN45" s="11"/>
       <c r="AO45" s="58"/>
-      <c r="AR45" s="70"/>
-      <c r="AS45" s="70"/>
-      <c r="AT45" s="70"/>
-      <c r="AU45" s="70"/>
+      <c r="AR45" s="69"/>
+      <c r="AS45" s="69"/>
+      <c r="AT45" s="69"/>
+      <c r="AU45" s="69"/>
       <c r="AV45" s="11"/>
       <c r="AW45" s="9"/>
       <c r="AX45" s="10"/>
@@ -10366,12 +10439,12 @@
       <c r="CD45" s="9"/>
       <c r="CE45" s="10"/>
       <c r="CF45" s="10"/>
-      <c r="CG45" s="67"/>
+      <c r="CG45" s="66"/>
     </row>
     <row r="46" spans="1:85" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A46" s="41"/>
-      <c r="B46" s="100"/>
-      <c r="C46" s="106"/>
+      <c r="B46" s="99"/>
+      <c r="C46" s="105"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
@@ -10459,10 +10532,10 @@
       <c r="A47" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="B47" s="99">
+      <c r="B47" s="98">
         <v>3</v>
       </c>
-      <c r="C47" s="105"/>
+      <c r="C47" s="104"/>
       <c r="D47" s="10"/>
       <c r="E47" s="10"/>
       <c r="F47" s="10"/>
@@ -10506,9 +10579,9 @@
       <c r="AR47" s="10"/>
       <c r="AS47" s="10"/>
       <c r="AT47" s="10"/>
-      <c r="AV47" s="70"/>
-      <c r="AW47" s="70"/>
-      <c r="AX47" s="70"/>
+      <c r="AV47" s="69"/>
+      <c r="AW47" s="69"/>
+      <c r="AX47" s="69"/>
       <c r="AY47" s="10"/>
       <c r="AZ47" s="10"/>
       <c r="BA47" s="10"/>
@@ -10543,12 +10616,12 @@
       <c r="CD47" s="9"/>
       <c r="CE47" s="10"/>
       <c r="CF47" s="10"/>
-      <c r="CG47" s="67"/>
+      <c r="CG47" s="66"/>
     </row>
     <row r="48" spans="1:85" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A48" s="41"/>
-      <c r="B48" s="100"/>
-      <c r="C48" s="106"/>
+      <c r="B48" s="99"/>
+      <c r="C48" s="105"/>
       <c r="D48" s="6"/>
       <c r="E48" s="6"/>
       <c r="F48" s="6"/>
@@ -10636,10 +10709,10 @@
       <c r="A49" s="40" t="s">
         <v>33</v>
       </c>
-      <c r="B49" s="99">
+      <c r="B49" s="98">
         <v>4</v>
       </c>
-      <c r="C49" s="105"/>
+      <c r="C49" s="104"/>
       <c r="D49" s="10"/>
       <c r="E49" s="10"/>
       <c r="F49" s="10"/>
@@ -10685,10 +10758,10 @@
       <c r="AU49" s="58"/>
       <c r="AV49" s="59"/>
       <c r="AW49" s="57"/>
-      <c r="AY49" s="88"/>
-      <c r="AZ49" s="88"/>
-      <c r="BA49" s="88"/>
-      <c r="BB49" s="88"/>
+      <c r="AY49" s="87"/>
+      <c r="AZ49" s="87"/>
+      <c r="BA49" s="87"/>
+      <c r="BB49" s="87"/>
       <c r="BC49" s="10"/>
       <c r="BD49" s="11"/>
       <c r="BE49" s="9"/>
@@ -10719,12 +10792,12 @@
       <c r="CD49" s="9"/>
       <c r="CE49" s="10"/>
       <c r="CF49" s="10"/>
-      <c r="CG49" s="67"/>
+      <c r="CG49" s="66"/>
     </row>
     <row r="50" spans="1:85" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A50" s="41"/>
-      <c r="B50" s="100"/>
-      <c r="C50" s="106"/>
+      <c r="B50" s="99"/>
+      <c r="C50" s="105"/>
       <c r="D50" s="6"/>
       <c r="E50" s="6"/>
       <c r="F50" s="6"/>
@@ -10812,10 +10885,10 @@
       <c r="A51" s="40" t="s">
         <v>37</v>
       </c>
-      <c r="B51" s="99">
+      <c r="B51" s="98">
         <v>4</v>
       </c>
-      <c r="C51" s="105"/>
+      <c r="C51" s="104"/>
       <c r="D51" s="10"/>
       <c r="E51" s="10"/>
       <c r="F51" s="10"/>
@@ -10866,10 +10939,10 @@
       <c r="AY51" s="10"/>
       <c r="AZ51" s="10"/>
       <c r="BA51" s="10"/>
-      <c r="BC51" s="88"/>
-      <c r="BD51" s="88"/>
-      <c r="BE51" s="88"/>
-      <c r="BF51" s="88"/>
+      <c r="BC51" s="87"/>
+      <c r="BD51" s="87"/>
+      <c r="BE51" s="87"/>
+      <c r="BF51" s="87"/>
       <c r="BG51" s="10"/>
       <c r="BH51" s="10"/>
       <c r="BI51" s="10"/>
@@ -10896,12 +10969,12 @@
       <c r="CD51" s="9"/>
       <c r="CE51" s="10"/>
       <c r="CF51" s="10"/>
-      <c r="CG51" s="67"/>
+      <c r="CG51" s="66"/>
     </row>
     <row r="52" spans="1:85" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A52" s="41"/>
-      <c r="B52" s="100"/>
-      <c r="C52" s="106"/>
+      <c r="B52" s="99"/>
+      <c r="C52" s="105"/>
       <c r="D52" s="6"/>
       <c r="E52" s="6"/>
       <c r="F52" s="6"/>
@@ -10989,10 +11062,10 @@
       <c r="A53" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="B53" s="99">
+      <c r="B53" s="98">
         <v>6</v>
       </c>
-      <c r="C53" s="105"/>
+      <c r="C53" s="104"/>
       <c r="D53" s="10"/>
       <c r="E53" s="10"/>
       <c r="F53" s="10"/>
@@ -11046,12 +11119,12 @@
       <c r="BC53" s="10"/>
       <c r="BD53" s="10"/>
       <c r="BE53" s="9"/>
-      <c r="BG53" s="70"/>
-      <c r="BH53" s="70"/>
-      <c r="BI53" s="70"/>
-      <c r="BJ53" s="70"/>
-      <c r="BK53" s="70"/>
-      <c r="BL53" s="70"/>
+      <c r="BG53" s="69"/>
+      <c r="BH53" s="69"/>
+      <c r="BI53" s="69"/>
+      <c r="BJ53" s="69"/>
+      <c r="BK53" s="69"/>
+      <c r="BL53" s="69"/>
       <c r="BM53" s="46"/>
       <c r="BN53" s="9"/>
       <c r="BO53" s="10"/>
@@ -11072,12 +11145,12 @@
       <c r="CD53" s="9"/>
       <c r="CE53" s="10"/>
       <c r="CF53" s="10"/>
-      <c r="CG53" s="67"/>
+      <c r="CG53" s="66"/>
     </row>
     <row r="54" spans="1:85" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A54" s="41"/>
-      <c r="B54" s="100"/>
-      <c r="C54" s="106"/>
+      <c r="B54" s="99"/>
+      <c r="C54" s="105"/>
       <c r="D54" s="6"/>
       <c r="E54" s="6"/>
       <c r="F54" s="6"/>
@@ -11165,10 +11238,10 @@
       <c r="A55" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="B55" s="99">
+      <c r="B55" s="98">
         <v>2</v>
       </c>
-      <c r="C55" s="105"/>
+      <c r="C55" s="104"/>
       <c r="D55" s="10"/>
       <c r="E55" s="10"/>
       <c r="F55" s="10"/>
@@ -11221,7 +11294,7 @@
       <c r="BA55" s="10"/>
       <c r="BB55" s="10"/>
       <c r="BC55" s="10"/>
-      <c r="BE55" s="61"/>
+      <c r="BE55" s="60"/>
       <c r="BF55" s="18"/>
       <c r="BG55" s="58"/>
       <c r="BH55" s="10"/>
@@ -11229,8 +11302,8 @@
       <c r="BJ55" s="10"/>
       <c r="BK55" s="10"/>
       <c r="BM55" s="46"/>
-      <c r="BN55" s="73"/>
-      <c r="BO55" s="72"/>
+      <c r="BN55" s="72"/>
+      <c r="BO55" s="71"/>
       <c r="BP55" s="10"/>
       <c r="BQ55" s="10"/>
       <c r="BR55" s="10"/>
@@ -11248,12 +11321,12 @@
       <c r="CD55" s="9"/>
       <c r="CE55" s="10"/>
       <c r="CF55" s="10"/>
-      <c r="CG55" s="67"/>
+      <c r="CG55" s="66"/>
     </row>
     <row r="56" spans="1:85" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A56" s="41"/>
-      <c r="B56" s="100"/>
-      <c r="C56" s="106"/>
+      <c r="B56" s="99"/>
+      <c r="C56" s="105"/>
       <c r="D56" s="6"/>
       <c r="E56" s="6"/>
       <c r="F56" s="6"/>
@@ -11341,10 +11414,10 @@
       <c r="A57" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="B57" s="99">
+      <c r="B57" s="98">
         <v>3</v>
       </c>
-      <c r="C57" s="105"/>
+      <c r="C57" s="104"/>
       <c r="D57" s="10"/>
       <c r="E57" s="10"/>
       <c r="F57" s="10"/>
@@ -11406,9 +11479,9 @@
       <c r="BJ57" s="10"/>
       <c r="BL57" s="58"/>
       <c r="BM57" s="46"/>
-      <c r="BP57" s="70"/>
-      <c r="BQ57" s="70"/>
-      <c r="BR57" s="70"/>
+      <c r="BP57" s="69"/>
+      <c r="BQ57" s="69"/>
+      <c r="BR57" s="69"/>
       <c r="BS57" s="10"/>
       <c r="BU57" s="11"/>
       <c r="BV57" s="9"/>
@@ -11422,12 +11495,12 @@
       <c r="CD57" s="9"/>
       <c r="CE57" s="10"/>
       <c r="CF57" s="10"/>
-      <c r="CG57" s="67"/>
+      <c r="CG57" s="66"/>
     </row>
     <row r="58" spans="1:85" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A58" s="41"/>
-      <c r="B58" s="100"/>
-      <c r="C58" s="106"/>
+      <c r="B58" s="99"/>
+      <c r="C58" s="105"/>
       <c r="D58" s="6"/>
       <c r="E58" s="6"/>
       <c r="F58" s="6"/>
@@ -11515,10 +11588,10 @@
       <c r="A59" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="B59" s="99">
+      <c r="B59" s="98">
         <v>3</v>
       </c>
-      <c r="C59" s="105"/>
+      <c r="C59" s="104"/>
       <c r="D59" s="10"/>
       <c r="E59" s="10"/>
       <c r="F59" s="10"/>
@@ -11585,9 +11658,9 @@
       <c r="BO59" s="10"/>
       <c r="BP59" s="10"/>
       <c r="BQ59" s="10"/>
-      <c r="BU59" s="70"/>
-      <c r="BV59" s="70"/>
-      <c r="BW59" s="70"/>
+      <c r="BU59" s="69"/>
+      <c r="BV59" s="69"/>
+      <c r="BW59" s="69"/>
       <c r="BX59" s="10"/>
       <c r="BY59" s="10"/>
       <c r="BZ59" s="10"/>
@@ -11597,12 +11670,12 @@
       <c r="CD59" s="9"/>
       <c r="CE59" s="10"/>
       <c r="CF59" s="10"/>
-      <c r="CG59" s="67"/>
+      <c r="CG59" s="66"/>
     </row>
     <row r="60" spans="1:85" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A60" s="41"/>
-      <c r="B60" s="100"/>
-      <c r="C60" s="106"/>
+      <c r="B60" s="99"/>
+      <c r="C60" s="105"/>
       <c r="D60" s="6"/>
       <c r="E60" s="6"/>
       <c r="F60" s="6"/>
@@ -11690,10 +11763,10 @@
       <c r="A61" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="B61" s="99">
+      <c r="B61" s="98">
         <v>3</v>
       </c>
-      <c r="C61" s="105"/>
+      <c r="C61" s="104"/>
       <c r="D61" s="10"/>
       <c r="E61" s="10"/>
       <c r="F61" s="10"/>
@@ -11763,21 +11836,21 @@
       <c r="BS61" s="10"/>
       <c r="BT61" s="10"/>
       <c r="BU61" s="11"/>
-      <c r="BX61" s="70"/>
-      <c r="BY61" s="88"/>
-      <c r="BZ61" s="88"/>
+      <c r="BX61" s="69"/>
+      <c r="BY61" s="87"/>
+      <c r="BZ61" s="87"/>
       <c r="CA61" s="10"/>
       <c r="CB61" s="10"/>
       <c r="CC61" s="22"/>
       <c r="CD61" s="9"/>
       <c r="CE61" s="10"/>
       <c r="CF61" s="10"/>
-      <c r="CG61" s="67"/>
+      <c r="CG61" s="66"/>
     </row>
     <row r="62" spans="1:85" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A62" s="41"/>
-      <c r="B62" s="100"/>
-      <c r="C62" s="106"/>
+      <c r="B62" s="99"/>
+      <c r="C62" s="105"/>
       <c r="D62" s="6"/>
       <c r="E62" s="6"/>
       <c r="F62" s="6"/>
@@ -11865,10 +11938,10 @@
       <c r="A63" s="40" t="s">
         <v>36</v>
       </c>
-      <c r="B63" s="99">
+      <c r="B63" s="98">
         <v>2</v>
       </c>
-      <c r="C63" s="105"/>
+      <c r="C63" s="104"/>
       <c r="D63" s="10"/>
       <c r="E63" s="10"/>
       <c r="F63" s="10"/>
@@ -11940,18 +12013,18 @@
       <c r="BT63" s="10"/>
       <c r="BV63" s="9"/>
       <c r="BW63" s="10"/>
-      <c r="CA63" s="70"/>
-      <c r="CB63" s="70"/>
+      <c r="CA63" s="69"/>
+      <c r="CB63" s="69"/>
       <c r="CC63" s="22"/>
       <c r="CD63" s="9"/>
       <c r="CE63" s="10"/>
       <c r="CF63" s="10"/>
-      <c r="CG63" s="67"/>
+      <c r="CG63" s="66"/>
     </row>
     <row r="64" spans="1:85" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A64" s="41"/>
-      <c r="B64" s="100"/>
-      <c r="C64" s="106"/>
+      <c r="B64" s="99"/>
+      <c r="C64" s="105"/>
       <c r="D64" s="6"/>
       <c r="E64" s="6"/>
       <c r="F64" s="6"/>
@@ -12039,10 +12112,10 @@
       <c r="A65" s="40" t="s">
         <v>57</v>
       </c>
-      <c r="B65" s="99">
+      <c r="B65" s="98">
         <v>2</v>
       </c>
-      <c r="C65" s="105"/>
+      <c r="C65" s="104"/>
       <c r="D65" s="10"/>
       <c r="E65" s="10"/>
       <c r="F65" s="10"/>
@@ -12116,16 +12189,16 @@
       <c r="BV65" s="9"/>
       <c r="BX65" s="58"/>
       <c r="BY65" s="58"/>
-      <c r="CC65" s="70"/>
-      <c r="CD65" s="70"/>
+      <c r="CC65" s="69"/>
+      <c r="CD65" s="69"/>
       <c r="CE65" s="10"/>
       <c r="CF65" s="10"/>
-      <c r="CG65" s="67"/>
+      <c r="CG65" s="66"/>
     </row>
     <row r="66" spans="1:85" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A66" s="41"/>
-      <c r="B66" s="100"/>
-      <c r="C66" s="106"/>
+      <c r="B66" s="99"/>
+      <c r="C66" s="105"/>
       <c r="D66" s="6"/>
       <c r="E66" s="6"/>
       <c r="F66" s="6"/>
@@ -12213,10 +12286,10 @@
       <c r="A67" s="40" t="s">
         <v>38</v>
       </c>
-      <c r="B67" s="99">
+      <c r="B67" s="98">
         <v>3</v>
       </c>
-      <c r="C67" s="105"/>
+      <c r="C67" s="104"/>
       <c r="D67" s="10"/>
       <c r="E67" s="10"/>
       <c r="F67" s="10"/>
@@ -12296,190 +12369,190 @@
       <c r="CB67" s="10"/>
       <c r="CC67" s="22"/>
       <c r="CD67" s="10"/>
-      <c r="CE67" s="70"/>
-      <c r="CF67" s="70"/>
-      <c r="CG67" s="70"/>
+      <c r="CE67" s="69"/>
+      <c r="CF67" s="69"/>
+      <c r="CG67" s="69"/>
     </row>
     <row r="68" spans="1:85" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A68" s="40"/>
-      <c r="B68" s="100"/>
-      <c r="C68" s="106"/>
-      <c r="D68" s="95"/>
-      <c r="E68" s="95"/>
-      <c r="F68" s="95"/>
-      <c r="G68" s="69"/>
-      <c r="H68" s="89"/>
-      <c r="I68" s="95"/>
-      <c r="J68" s="95"/>
-      <c r="K68" s="95"/>
-      <c r="L68" s="95"/>
-      <c r="M68" s="95"/>
-      <c r="N68" s="95"/>
-      <c r="O68" s="69"/>
-      <c r="P68" s="89"/>
-      <c r="Q68" s="95"/>
-      <c r="R68" s="95"/>
-      <c r="S68" s="95"/>
-      <c r="T68" s="95"/>
-      <c r="U68" s="95"/>
-      <c r="V68" s="95"/>
-      <c r="W68" s="69"/>
+      <c r="B68" s="99"/>
+      <c r="C68" s="105"/>
+      <c r="D68" s="94"/>
+      <c r="E68" s="94"/>
+      <c r="F68" s="94"/>
+      <c r="G68" s="68"/>
+      <c r="H68" s="88"/>
+      <c r="I68" s="94"/>
+      <c r="J68" s="94"/>
+      <c r="K68" s="94"/>
+      <c r="L68" s="94"/>
+      <c r="M68" s="94"/>
+      <c r="N68" s="94"/>
+      <c r="O68" s="68"/>
+      <c r="P68" s="88"/>
+      <c r="Q68" s="94"/>
+      <c r="R68" s="94"/>
+      <c r="S68" s="94"/>
+      <c r="T68" s="94"/>
+      <c r="U68" s="94"/>
+      <c r="V68" s="94"/>
+      <c r="W68" s="68"/>
       <c r="X68" s="46"/>
-      <c r="Y68" s="89"/>
-      <c r="Z68" s="95"/>
-      <c r="AA68" s="95"/>
-      <c r="AB68" s="95"/>
-      <c r="AC68" s="95"/>
-      <c r="AD68" s="95"/>
-      <c r="AE68" s="95"/>
-      <c r="AF68" s="69"/>
-      <c r="AG68" s="89"/>
-      <c r="AH68" s="95"/>
-      <c r="AI68" s="95"/>
-      <c r="AJ68" s="95"/>
-      <c r="AK68" s="95"/>
-      <c r="AL68" s="95"/>
-      <c r="AM68" s="95"/>
-      <c r="AN68" s="69"/>
-      <c r="AO68" s="89"/>
-      <c r="AP68" s="95"/>
-      <c r="AQ68" s="95"/>
-      <c r="AR68" s="95"/>
-      <c r="AS68" s="95"/>
-      <c r="AT68" s="95"/>
-      <c r="AU68" s="95"/>
-      <c r="AV68" s="69"/>
-      <c r="AW68" s="89"/>
-      <c r="AX68" s="95"/>
-      <c r="AY68" s="95"/>
-      <c r="AZ68" s="95"/>
-      <c r="BA68" s="95"/>
-      <c r="BB68" s="95"/>
-      <c r="BC68" s="95"/>
-      <c r="BD68" s="69"/>
-      <c r="BE68" s="89"/>
-      <c r="BF68" s="95"/>
-      <c r="BG68" s="95"/>
-      <c r="BH68" s="95"/>
-      <c r="BI68" s="95"/>
-      <c r="BJ68" s="95"/>
-      <c r="BK68" s="95"/>
-      <c r="BL68" s="69"/>
+      <c r="Y68" s="88"/>
+      <c r="Z68" s="94"/>
+      <c r="AA68" s="94"/>
+      <c r="AB68" s="94"/>
+      <c r="AC68" s="94"/>
+      <c r="AD68" s="94"/>
+      <c r="AE68" s="94"/>
+      <c r="AF68" s="68"/>
+      <c r="AG68" s="88"/>
+      <c r="AH68" s="94"/>
+      <c r="AI68" s="94"/>
+      <c r="AJ68" s="94"/>
+      <c r="AK68" s="94"/>
+      <c r="AL68" s="94"/>
+      <c r="AM68" s="94"/>
+      <c r="AN68" s="68"/>
+      <c r="AO68" s="88"/>
+      <c r="AP68" s="94"/>
+      <c r="AQ68" s="94"/>
+      <c r="AR68" s="94"/>
+      <c r="AS68" s="94"/>
+      <c r="AT68" s="94"/>
+      <c r="AU68" s="94"/>
+      <c r="AV68" s="68"/>
+      <c r="AW68" s="88"/>
+      <c r="AX68" s="94"/>
+      <c r="AY68" s="94"/>
+      <c r="AZ68" s="94"/>
+      <c r="BA68" s="94"/>
+      <c r="BB68" s="94"/>
+      <c r="BC68" s="94"/>
+      <c r="BD68" s="68"/>
+      <c r="BE68" s="88"/>
+      <c r="BF68" s="94"/>
+      <c r="BG68" s="94"/>
+      <c r="BH68" s="94"/>
+      <c r="BI68" s="94"/>
+      <c r="BJ68" s="94"/>
+      <c r="BK68" s="94"/>
+      <c r="BL68" s="68"/>
       <c r="BM68" s="46"/>
-      <c r="BN68" s="89"/>
-      <c r="BO68" s="95"/>
-      <c r="BP68" s="95"/>
-      <c r="BQ68" s="95"/>
-      <c r="BR68" s="95"/>
-      <c r="BS68" s="95"/>
-      <c r="BT68" s="95"/>
-      <c r="BU68" s="69"/>
-      <c r="BV68" s="89"/>
-      <c r="BW68" s="95"/>
-      <c r="BX68" s="95"/>
-      <c r="CC68" s="96"/>
-      <c r="CD68" s="95"/>
-      <c r="CE68" s="95"/>
-      <c r="CF68" s="95"/>
+      <c r="BN68" s="88"/>
+      <c r="BO68" s="94"/>
+      <c r="BP68" s="94"/>
+      <c r="BQ68" s="94"/>
+      <c r="BR68" s="94"/>
+      <c r="BS68" s="94"/>
+      <c r="BT68" s="94"/>
+      <c r="BU68" s="68"/>
+      <c r="BV68" s="88"/>
+      <c r="BW68" s="94"/>
+      <c r="BX68" s="94"/>
+      <c r="CC68" s="95"/>
+      <c r="CD68" s="94"/>
+      <c r="CE68" s="94"/>
+      <c r="CF68" s="94"/>
       <c r="CG68" s="3"/>
     </row>
     <row r="69" spans="1:85" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A69" s="92" t="s">
+      <c r="A69" s="91" t="s">
         <v>43</v>
       </c>
-      <c r="B69" s="93"/>
-      <c r="C69" s="93"/>
-      <c r="D69" s="93"/>
-      <c r="E69" s="93"/>
-      <c r="F69" s="93"/>
-      <c r="G69" s="94"/>
-      <c r="H69" s="93"/>
-      <c r="I69" s="93"/>
-      <c r="J69" s="93"/>
-      <c r="K69" s="93"/>
-      <c r="L69" s="93"/>
-      <c r="M69" s="93"/>
-      <c r="N69" s="93"/>
-      <c r="O69" s="93"/>
-      <c r="P69" s="93"/>
-      <c r="Q69" s="93"/>
-      <c r="R69" s="93"/>
-      <c r="S69" s="93"/>
-      <c r="T69" s="93"/>
-      <c r="U69" s="93"/>
-      <c r="V69" s="93"/>
-      <c r="W69" s="93"/>
+      <c r="B69" s="92"/>
+      <c r="C69" s="92"/>
+      <c r="D69" s="92"/>
+      <c r="E69" s="92"/>
+      <c r="F69" s="92"/>
+      <c r="G69" s="93"/>
+      <c r="H69" s="92"/>
+      <c r="I69" s="92"/>
+      <c r="J69" s="92"/>
+      <c r="K69" s="92"/>
+      <c r="L69" s="92"/>
+      <c r="M69" s="92"/>
+      <c r="N69" s="92"/>
+      <c r="O69" s="92"/>
+      <c r="P69" s="92"/>
+      <c r="Q69" s="92"/>
+      <c r="R69" s="92"/>
+      <c r="S69" s="92"/>
+      <c r="T69" s="92"/>
+      <c r="U69" s="92"/>
+      <c r="V69" s="92"/>
+      <c r="W69" s="92"/>
       <c r="X69" s="46"/>
-      <c r="Y69" s="93"/>
-      <c r="Z69" s="93"/>
-      <c r="AA69" s="93"/>
-      <c r="AB69" s="93"/>
-      <c r="AC69" s="93"/>
-      <c r="AD69" s="93"/>
-      <c r="AE69" s="93"/>
-      <c r="AF69" s="93"/>
-      <c r="AG69" s="93"/>
-      <c r="AH69" s="93"/>
-      <c r="AI69" s="93"/>
-      <c r="AJ69" s="93"/>
-      <c r="AK69" s="93"/>
-      <c r="AL69" s="93"/>
-      <c r="AM69" s="93"/>
-      <c r="AN69" s="94"/>
+      <c r="Y69" s="92"/>
+      <c r="Z69" s="92"/>
+      <c r="AA69" s="92"/>
+      <c r="AB69" s="92"/>
+      <c r="AC69" s="92"/>
+      <c r="AD69" s="92"/>
+      <c r="AE69" s="92"/>
+      <c r="AF69" s="92"/>
+      <c r="AG69" s="92"/>
+      <c r="AH69" s="92"/>
+      <c r="AI69" s="92"/>
+      <c r="AJ69" s="92"/>
+      <c r="AK69" s="92"/>
+      <c r="AL69" s="92"/>
+      <c r="AM69" s="92"/>
+      <c r="AN69" s="93"/>
       <c r="AO69" s="33"/>
-      <c r="AP69" s="90"/>
-      <c r="AQ69" s="90"/>
-      <c r="AR69" s="90"/>
-      <c r="AS69" s="90"/>
-      <c r="AT69" s="90"/>
-      <c r="AU69" s="90"/>
-      <c r="AV69" s="90"/>
-      <c r="AW69" s="90"/>
-      <c r="AX69" s="90"/>
-      <c r="AY69" s="90"/>
-      <c r="AZ69" s="90"/>
-      <c r="BA69" s="90"/>
-      <c r="BB69" s="90"/>
-      <c r="BC69" s="90"/>
-      <c r="BD69" s="90"/>
-      <c r="BE69" s="90"/>
-      <c r="BF69" s="90"/>
-      <c r="BG69" s="90"/>
-      <c r="BH69" s="90"/>
-      <c r="BI69" s="90"/>
-      <c r="BJ69" s="90"/>
-      <c r="BK69" s="90"/>
-      <c r="BL69" s="90"/>
+      <c r="AP69" s="89"/>
+      <c r="AQ69" s="89"/>
+      <c r="AR69" s="89"/>
+      <c r="AS69" s="89"/>
+      <c r="AT69" s="89"/>
+      <c r="AU69" s="89"/>
+      <c r="AV69" s="89"/>
+      <c r="AW69" s="89"/>
+      <c r="AX69" s="89"/>
+      <c r="AY69" s="89"/>
+      <c r="AZ69" s="89"/>
+      <c r="BA69" s="89"/>
+      <c r="BB69" s="89"/>
+      <c r="BC69" s="89"/>
+      <c r="BD69" s="89"/>
+      <c r="BE69" s="89"/>
+      <c r="BF69" s="89"/>
+      <c r="BG69" s="89"/>
+      <c r="BH69" s="89"/>
+      <c r="BI69" s="89"/>
+      <c r="BJ69" s="89"/>
+      <c r="BK69" s="89"/>
+      <c r="BL69" s="89"/>
       <c r="BM69" s="46"/>
-      <c r="BN69" s="90"/>
-      <c r="BO69" s="90"/>
-      <c r="BP69" s="90"/>
-      <c r="BQ69" s="90"/>
-      <c r="BR69" s="90"/>
-      <c r="BS69" s="90"/>
-      <c r="BT69" s="90"/>
-      <c r="BU69" s="90"/>
-      <c r="BV69" s="90"/>
-      <c r="BW69" s="90"/>
-      <c r="BX69" s="90"/>
-      <c r="BY69" s="90"/>
-      <c r="BZ69" s="90"/>
-      <c r="CA69" s="90"/>
-      <c r="CB69" s="90"/>
+      <c r="BN69" s="89"/>
+      <c r="BO69" s="89"/>
+      <c r="BP69" s="89"/>
+      <c r="BQ69" s="89"/>
+      <c r="BR69" s="89"/>
+      <c r="BS69" s="89"/>
+      <c r="BT69" s="89"/>
+      <c r="BU69" s="89"/>
+      <c r="BV69" s="89"/>
+      <c r="BW69" s="89"/>
+      <c r="BX69" s="89"/>
+      <c r="BY69" s="89"/>
+      <c r="BZ69" s="89"/>
+      <c r="CA69" s="89"/>
+      <c r="CB69" s="89"/>
       <c r="CC69" s="34"/>
-      <c r="CD69" s="90"/>
-      <c r="CE69" s="90"/>
-      <c r="CF69" s="90"/>
-      <c r="CG69" s="91"/>
+      <c r="CD69" s="89"/>
+      <c r="CE69" s="89"/>
+      <c r="CF69" s="89"/>
+      <c r="CG69" s="90"/>
     </row>
     <row r="70" spans="1:85" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A70" s="40" t="s">
         <v>44</v>
       </c>
-      <c r="B70" s="99">
+      <c r="B70" s="98">
         <v>6</v>
       </c>
-      <c r="C70" s="103"/>
+      <c r="C70" s="102"/>
       <c r="D70" s="6"/>
       <c r="E70" s="6"/>
       <c r="F70" s="6"/>
@@ -12492,7 +12565,7 @@
       <c r="M70" s="6"/>
       <c r="N70" s="6"/>
       <c r="O70" s="16"/>
-      <c r="P70" s="98"/>
+      <c r="P70" s="97"/>
       <c r="Q70" s="6"/>
       <c r="R70" s="6"/>
       <c r="S70" s="6"/>
@@ -12505,7 +12578,7 @@
       <c r="Z70" s="6"/>
       <c r="AA70" s="6"/>
       <c r="AB70" s="6"/>
-      <c r="AC70" s="97"/>
+      <c r="AC70" s="96"/>
       <c r="AD70" s="6"/>
       <c r="AE70" s="6"/>
       <c r="AF70" s="16"/>
@@ -12514,8 +12587,8 @@
       <c r="AI70" s="6"/>
       <c r="AJ70" s="6"/>
       <c r="AK70" s="6"/>
-      <c r="AL70" s="97"/>
-      <c r="AM70" s="97"/>
+      <c r="AL70" s="96"/>
+      <c r="AM70" s="96"/>
       <c r="AN70" s="16"/>
       <c r="AO70" s="2"/>
       <c r="AP70" s="6"/>
@@ -12547,8 +12620,8 @@
       <c r="BP70" s="6"/>
       <c r="BQ70" s="6"/>
       <c r="BR70" s="6"/>
-      <c r="BS70" s="97"/>
-      <c r="BT70" s="97"/>
+      <c r="BS70" s="96"/>
+      <c r="BT70" s="96"/>
       <c r="BU70" s="16"/>
       <c r="BV70" s="2"/>
       <c r="BW70" s="6"/>
@@ -12565,8 +12638,8 @@
     </row>
     <row r="71" spans="1:85" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A71" s="40"/>
-      <c r="B71" s="100"/>
-      <c r="C71" s="104"/>
+      <c r="B71" s="99"/>
+      <c r="C71" s="103"/>
       <c r="D71" s="6"/>
       <c r="E71" s="6"/>
       <c r="F71" s="6"/>
@@ -12579,9 +12652,8 @@
       <c r="M71" s="6"/>
       <c r="N71" s="6"/>
       <c r="O71" s="16"/>
-      <c r="P71" s="136"/>
-      <c r="Q71" s="83"/>
-      <c r="R71" s="6"/>
+      <c r="Q71" s="82"/>
+      <c r="R71" s="135"/>
       <c r="S71" s="6"/>
       <c r="T71" s="6"/>
       <c r="U71" s="6"/>
@@ -12735,10 +12807,10 @@
       <c r="CD72" s="37"/>
       <c r="CE72" s="37"/>
       <c r="CF72" s="37"/>
-      <c r="CG72" s="68"/>
+      <c r="CG72" s="67"/>
     </row>
     <row r="73" spans="1:85" x14ac:dyDescent="0.35">
-      <c r="A73" s="101" t="s">
+      <c r="A73" s="100" t="s">
         <v>4</v>
       </c>
       <c r="B73" s="48">
@@ -12747,7 +12819,7 @@
       </c>
       <c r="C73" s="49">
         <f>SUM(C41:C70)+SUM(C17:C27)+SUM(C8:C14)</f>
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="D73" s="31"/>
       <c r="E73" s="31"/>
@@ -12830,10 +12902,10 @@
       <c r="CD73" s="13"/>
       <c r="CE73" s="13"/>
       <c r="CF73" s="13"/>
-      <c r="CG73" s="66"/>
+      <c r="CG73" s="65"/>
     </row>
     <row r="74" spans="1:85" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A74" s="102"/>
+      <c r="A74" s="101"/>
       <c r="B74" s="23" t="s">
         <v>2</v>
       </c>
@@ -13203,321 +13275,321 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="16384" width="8.6640625" style="75"/>
+    <col min="1" max="16384" width="8.6640625" style="74"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A1" s="81"/>
-      <c r="B1" s="78"/>
-      <c r="C1" s="78"/>
-      <c r="D1" s="78"/>
-      <c r="E1" s="78"/>
-      <c r="F1" s="78"/>
-      <c r="G1" s="78"/>
-      <c r="H1" s="78"/>
-      <c r="I1" s="78"/>
-      <c r="J1" s="78"/>
-      <c r="K1" s="78"/>
-      <c r="L1" s="78"/>
-      <c r="M1" s="78"/>
-      <c r="N1" s="78"/>
-      <c r="O1" s="78"/>
+      <c r="A1" s="80"/>
+      <c r="B1" s="77"/>
+      <c r="C1" s="77"/>
+      <c r="D1" s="77"/>
+      <c r="E1" s="77"/>
+      <c r="F1" s="77"/>
+      <c r="G1" s="77"/>
+      <c r="H1" s="77"/>
+      <c r="I1" s="77"/>
+      <c r="J1" s="77"/>
+      <c r="K1" s="77"/>
+      <c r="L1" s="77"/>
+      <c r="M1" s="77"/>
+      <c r="N1" s="77"/>
+      <c r="O1" s="77"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A2" s="78"/>
-      <c r="B2" s="78"/>
-      <c r="C2" s="78"/>
-      <c r="D2" s="78"/>
-      <c r="E2" s="78"/>
-      <c r="F2" s="78"/>
-      <c r="G2" s="78"/>
-      <c r="H2" s="78"/>
-      <c r="I2" s="78"/>
-      <c r="J2" s="78"/>
-      <c r="K2" s="78"/>
-      <c r="L2" s="78"/>
-      <c r="M2" s="78"/>
-      <c r="N2" s="78"/>
-      <c r="O2" s="78"/>
+      <c r="A2" s="77"/>
+      <c r="B2" s="77"/>
+      <c r="C2" s="77"/>
+      <c r="D2" s="77"/>
+      <c r="E2" s="77"/>
+      <c r="F2" s="77"/>
+      <c r="G2" s="77"/>
+      <c r="H2" s="77"/>
+      <c r="I2" s="77"/>
+      <c r="J2" s="77"/>
+      <c r="K2" s="77"/>
+      <c r="L2" s="77"/>
+      <c r="M2" s="77"/>
+      <c r="N2" s="77"/>
+      <c r="O2" s="77"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A3" s="77"/>
-      <c r="B3" s="80" t="s">
+      <c r="A3" s="76"/>
+      <c r="B3" s="79" t="s">
         <v>32</v>
       </c>
-      <c r="C3" s="82" t="s">
+      <c r="C3" s="81" t="s">
         <v>31</v>
       </c>
-      <c r="D3" s="82" t="s">
+      <c r="D3" s="81" t="s">
         <v>30</v>
       </c>
-      <c r="E3" s="82" t="s">
+      <c r="E3" s="81" t="s">
         <v>29</v>
       </c>
-      <c r="F3" s="82" t="s">
+      <c r="F3" s="81" t="s">
         <v>28</v>
       </c>
-      <c r="G3" s="82" t="s">
+      <c r="G3" s="81" t="s">
         <v>27</v>
       </c>
-      <c r="H3" s="80" t="s">
+      <c r="H3" s="79" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="82" t="s">
+      <c r="I3" s="81" t="s">
         <v>25</v>
       </c>
-      <c r="J3" s="82" t="s">
+      <c r="J3" s="81" t="s">
         <v>24</v>
       </c>
-      <c r="K3" s="82" t="s">
+      <c r="K3" s="81" t="s">
         <v>23</v>
       </c>
-      <c r="L3" s="78"/>
-      <c r="M3" s="78"/>
-      <c r="N3" s="78"/>
-      <c r="O3" s="78"/>
+      <c r="L3" s="77"/>
+      <c r="M3" s="77"/>
+      <c r="N3" s="77"/>
+      <c r="O3" s="77"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A4" s="77"/>
-      <c r="B4" s="77"/>
-      <c r="C4" s="76"/>
-      <c r="D4" s="76"/>
-      <c r="E4" s="76"/>
-      <c r="F4" s="76"/>
-      <c r="G4" s="76"/>
-      <c r="H4" s="77"/>
-      <c r="I4" s="76"/>
-      <c r="J4" s="76"/>
-      <c r="K4" s="76"/>
-      <c r="L4" s="78"/>
-      <c r="M4" s="78"/>
-      <c r="N4" s="78"/>
-      <c r="O4" s="78"/>
+      <c r="A4" s="76"/>
+      <c r="B4" s="76"/>
+      <c r="C4" s="75"/>
+      <c r="D4" s="75"/>
+      <c r="E4" s="75"/>
+      <c r="F4" s="75"/>
+      <c r="G4" s="75"/>
+      <c r="H4" s="76"/>
+      <c r="I4" s="75"/>
+      <c r="J4" s="75"/>
+      <c r="K4" s="75"/>
+      <c r="L4" s="77"/>
+      <c r="M4" s="77"/>
+      <c r="N4" s="77"/>
+      <c r="O4" s="77"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A5" s="77"/>
-      <c r="B5" s="77"/>
-      <c r="C5" s="76"/>
-      <c r="D5" s="76"/>
-      <c r="E5" s="76"/>
-      <c r="F5" s="76"/>
-      <c r="G5" s="76"/>
-      <c r="H5" s="77"/>
-      <c r="I5" s="76"/>
-      <c r="J5" s="76"/>
-      <c r="K5" s="76"/>
-      <c r="L5" s="78"/>
-      <c r="M5" s="78"/>
-      <c r="N5" s="78"/>
-      <c r="O5" s="78"/>
+      <c r="A5" s="76"/>
+      <c r="B5" s="76"/>
+      <c r="C5" s="75"/>
+      <c r="D5" s="75"/>
+      <c r="E5" s="75"/>
+      <c r="F5" s="75"/>
+      <c r="G5" s="75"/>
+      <c r="H5" s="76"/>
+      <c r="I5" s="75"/>
+      <c r="J5" s="75"/>
+      <c r="K5" s="75"/>
+      <c r="L5" s="77"/>
+      <c r="M5" s="77"/>
+      <c r="N5" s="77"/>
+      <c r="O5" s="77"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A6" s="77"/>
-      <c r="B6" s="77"/>
-      <c r="C6" s="76"/>
-      <c r="D6" s="76"/>
-      <c r="E6" s="76"/>
-      <c r="F6" s="76"/>
-      <c r="G6" s="76"/>
-      <c r="H6" s="77"/>
-      <c r="I6" s="76"/>
-      <c r="J6" s="76"/>
-      <c r="K6" s="76"/>
-      <c r="L6" s="78"/>
-      <c r="M6" s="78"/>
-      <c r="N6" s="78"/>
-      <c r="O6" s="78"/>
+      <c r="A6" s="76"/>
+      <c r="B6" s="76"/>
+      <c r="C6" s="75"/>
+      <c r="D6" s="75"/>
+      <c r="E6" s="75"/>
+      <c r="F6" s="75"/>
+      <c r="G6" s="75"/>
+      <c r="H6" s="76"/>
+      <c r="I6" s="75"/>
+      <c r="J6" s="75"/>
+      <c r="K6" s="75"/>
+      <c r="L6" s="77"/>
+      <c r="M6" s="77"/>
+      <c r="N6" s="77"/>
+      <c r="O6" s="77"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A7" s="77"/>
-      <c r="B7" s="77"/>
-      <c r="C7" s="76"/>
-      <c r="D7" s="76"/>
-      <c r="E7" s="76"/>
-      <c r="F7" s="76"/>
-      <c r="G7" s="76"/>
-      <c r="H7" s="77"/>
-      <c r="I7" s="76"/>
-      <c r="J7" s="76"/>
-      <c r="K7" s="76"/>
-      <c r="L7" s="78"/>
-      <c r="M7" s="78"/>
-      <c r="N7" s="78"/>
-      <c r="O7" s="78"/>
+      <c r="A7" s="76"/>
+      <c r="B7" s="76"/>
+      <c r="C7" s="75"/>
+      <c r="D7" s="75"/>
+      <c r="E7" s="75"/>
+      <c r="F7" s="75"/>
+      <c r="G7" s="75"/>
+      <c r="H7" s="76"/>
+      <c r="I7" s="75"/>
+      <c r="J7" s="75"/>
+      <c r="K7" s="75"/>
+      <c r="L7" s="77"/>
+      <c r="M7" s="77"/>
+      <c r="N7" s="77"/>
+      <c r="O7" s="77"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A8" s="77"/>
-      <c r="B8" s="77"/>
-      <c r="C8" s="76"/>
-      <c r="D8" s="76"/>
-      <c r="E8" s="76"/>
-      <c r="F8" s="76"/>
-      <c r="G8" s="76"/>
-      <c r="H8" s="77"/>
-      <c r="I8" s="76"/>
-      <c r="J8" s="76"/>
-      <c r="K8" s="76"/>
-      <c r="L8" s="78"/>
-      <c r="M8" s="78"/>
-      <c r="N8" s="78"/>
-      <c r="O8" s="78"/>
+      <c r="A8" s="76"/>
+      <c r="B8" s="76"/>
+      <c r="C8" s="75"/>
+      <c r="D8" s="75"/>
+      <c r="E8" s="75"/>
+      <c r="F8" s="75"/>
+      <c r="G8" s="75"/>
+      <c r="H8" s="76"/>
+      <c r="I8" s="75"/>
+      <c r="J8" s="75"/>
+      <c r="K8" s="75"/>
+      <c r="L8" s="77"/>
+      <c r="M8" s="77"/>
+      <c r="N8" s="77"/>
+      <c r="O8" s="77"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A9" s="77"/>
-      <c r="B9" s="77"/>
-      <c r="C9" s="76"/>
-      <c r="D9" s="76"/>
-      <c r="E9" s="76"/>
-      <c r="F9" s="76"/>
-      <c r="G9" s="76"/>
-      <c r="H9" s="77"/>
-      <c r="I9" s="76"/>
-      <c r="J9" s="76"/>
-      <c r="K9" s="76"/>
-      <c r="L9" s="78"/>
-      <c r="M9" s="78"/>
-      <c r="N9" s="78"/>
-      <c r="O9" s="78"/>
+      <c r="A9" s="76"/>
+      <c r="B9" s="76"/>
+      <c r="C9" s="75"/>
+      <c r="D9" s="75"/>
+      <c r="E9" s="75"/>
+      <c r="F9" s="75"/>
+      <c r="G9" s="75"/>
+      <c r="H9" s="76"/>
+      <c r="I9" s="75"/>
+      <c r="J9" s="75"/>
+      <c r="K9" s="75"/>
+      <c r="L9" s="77"/>
+      <c r="M9" s="77"/>
+      <c r="N9" s="77"/>
+      <c r="O9" s="77"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A10" s="77"/>
-      <c r="B10" s="77"/>
-      <c r="C10" s="76"/>
-      <c r="D10" s="76"/>
-      <c r="E10" s="76"/>
-      <c r="F10" s="76"/>
-      <c r="G10" s="76"/>
-      <c r="H10" s="77"/>
-      <c r="I10" s="76"/>
-      <c r="J10" s="76"/>
-      <c r="K10" s="76"/>
-      <c r="L10" s="78"/>
-      <c r="M10" s="78"/>
-      <c r="N10" s="78"/>
-      <c r="O10" s="78"/>
+      <c r="A10" s="76"/>
+      <c r="B10" s="76"/>
+      <c r="C10" s="75"/>
+      <c r="D10" s="75"/>
+      <c r="E10" s="75"/>
+      <c r="F10" s="75"/>
+      <c r="G10" s="75"/>
+      <c r="H10" s="76"/>
+      <c r="I10" s="75"/>
+      <c r="J10" s="75"/>
+      <c r="K10" s="75"/>
+      <c r="L10" s="77"/>
+      <c r="M10" s="77"/>
+      <c r="N10" s="77"/>
+      <c r="O10" s="77"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A11" s="77"/>
-      <c r="B11" s="77"/>
-      <c r="C11" s="76"/>
-      <c r="D11" s="76"/>
-      <c r="E11" s="76"/>
-      <c r="F11" s="76"/>
-      <c r="G11" s="76"/>
-      <c r="H11" s="77"/>
-      <c r="I11" s="76"/>
-      <c r="J11" s="76"/>
-      <c r="K11" s="76"/>
-      <c r="L11" s="78"/>
-      <c r="M11" s="78"/>
-      <c r="N11" s="78"/>
-      <c r="O11" s="78"/>
+      <c r="A11" s="76"/>
+      <c r="B11" s="76"/>
+      <c r="C11" s="75"/>
+      <c r="D11" s="75"/>
+      <c r="E11" s="75"/>
+      <c r="F11" s="75"/>
+      <c r="G11" s="75"/>
+      <c r="H11" s="76"/>
+      <c r="I11" s="75"/>
+      <c r="J11" s="75"/>
+      <c r="K11" s="75"/>
+      <c r="L11" s="77"/>
+      <c r="M11" s="77"/>
+      <c r="N11" s="77"/>
+      <c r="O11" s="77"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A12" s="77"/>
-      <c r="B12" s="77"/>
-      <c r="C12" s="76"/>
-      <c r="D12" s="76"/>
-      <c r="E12" s="76"/>
-      <c r="F12" s="76"/>
-      <c r="G12" s="76"/>
-      <c r="H12" s="77"/>
-      <c r="I12" s="76"/>
-      <c r="J12" s="76"/>
-      <c r="K12" s="76"/>
-      <c r="L12" s="78"/>
-      <c r="M12" s="78"/>
-      <c r="N12" s="78"/>
-      <c r="O12" s="78"/>
+      <c r="A12" s="76"/>
+      <c r="B12" s="76"/>
+      <c r="C12" s="75"/>
+      <c r="D12" s="75"/>
+      <c r="E12" s="75"/>
+      <c r="F12" s="75"/>
+      <c r="G12" s="75"/>
+      <c r="H12" s="76"/>
+      <c r="I12" s="75"/>
+      <c r="J12" s="75"/>
+      <c r="K12" s="75"/>
+      <c r="L12" s="77"/>
+      <c r="M12" s="77"/>
+      <c r="N12" s="77"/>
+      <c r="O12" s="77"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A13" s="77"/>
-      <c r="B13" s="77"/>
-      <c r="C13" s="76"/>
-      <c r="D13" s="76"/>
-      <c r="E13" s="76"/>
-      <c r="F13" s="76"/>
-      <c r="G13" s="76"/>
-      <c r="H13" s="77"/>
-      <c r="I13" s="76"/>
-      <c r="J13" s="76"/>
-      <c r="K13" s="76"/>
-      <c r="L13" s="78"/>
-      <c r="M13" s="78"/>
-      <c r="N13" s="78"/>
-      <c r="O13" s="78"/>
+      <c r="A13" s="76"/>
+      <c r="B13" s="76"/>
+      <c r="C13" s="75"/>
+      <c r="D13" s="75"/>
+      <c r="E13" s="75"/>
+      <c r="F13" s="75"/>
+      <c r="G13" s="75"/>
+      <c r="H13" s="76"/>
+      <c r="I13" s="75"/>
+      <c r="J13" s="75"/>
+      <c r="K13" s="75"/>
+      <c r="L13" s="77"/>
+      <c r="M13" s="77"/>
+      <c r="N13" s="77"/>
+      <c r="O13" s="77"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A14" s="78"/>
-      <c r="B14" s="78"/>
-      <c r="C14" s="78"/>
-      <c r="D14" s="78"/>
-      <c r="E14" s="78"/>
-      <c r="F14" s="78"/>
-      <c r="G14" s="78"/>
-      <c r="H14" s="78"/>
-      <c r="I14" s="78"/>
-      <c r="J14" s="78"/>
-      <c r="K14" s="78"/>
-      <c r="L14" s="78"/>
-      <c r="M14" s="78"/>
-      <c r="N14" s="78"/>
-      <c r="O14" s="78"/>
+      <c r="A14" s="77"/>
+      <c r="B14" s="77"/>
+      <c r="C14" s="77"/>
+      <c r="D14" s="77"/>
+      <c r="E14" s="77"/>
+      <c r="F14" s="77"/>
+      <c r="G14" s="77"/>
+      <c r="H14" s="77"/>
+      <c r="I14" s="77"/>
+      <c r="J14" s="77"/>
+      <c r="K14" s="77"/>
+      <c r="L14" s="77"/>
+      <c r="M14" s="77"/>
+      <c r="N14" s="77"/>
+      <c r="O14" s="77"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A15" s="78"/>
-      <c r="B15" s="78"/>
-      <c r="C15" s="78"/>
-      <c r="D15" s="78"/>
-      <c r="E15" s="78"/>
-      <c r="F15" s="78"/>
-      <c r="G15" s="78"/>
-      <c r="H15" s="78"/>
-      <c r="I15" s="78"/>
-      <c r="J15" s="78"/>
-      <c r="K15" s="78"/>
-      <c r="L15" s="78"/>
-      <c r="M15" s="78"/>
-      <c r="N15" s="78"/>
-      <c r="O15" s="78"/>
+      <c r="A15" s="77"/>
+      <c r="B15" s="77"/>
+      <c r="C15" s="77"/>
+      <c r="D15" s="77"/>
+      <c r="E15" s="77"/>
+      <c r="F15" s="77"/>
+      <c r="G15" s="77"/>
+      <c r="H15" s="77"/>
+      <c r="I15" s="77"/>
+      <c r="J15" s="77"/>
+      <c r="K15" s="77"/>
+      <c r="L15" s="77"/>
+      <c r="M15" s="77"/>
+      <c r="N15" s="77"/>
+      <c r="O15" s="77"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A16" s="78"/>
-      <c r="B16" s="78"/>
-      <c r="C16" s="78"/>
-      <c r="D16" s="78"/>
-      <c r="E16" s="78"/>
-      <c r="F16" s="78"/>
-      <c r="G16" s="78"/>
-      <c r="H16" s="78"/>
-      <c r="I16" s="78"/>
-      <c r="J16" s="78"/>
-      <c r="K16" s="78"/>
-      <c r="L16" s="78"/>
-      <c r="M16" s="78"/>
-      <c r="N16" s="78"/>
-      <c r="O16" s="78"/>
+      <c r="A16" s="77"/>
+      <c r="B16" s="77"/>
+      <c r="C16" s="77"/>
+      <c r="D16" s="77"/>
+      <c r="E16" s="77"/>
+      <c r="F16" s="77"/>
+      <c r="G16" s="77"/>
+      <c r="H16" s="77"/>
+      <c r="I16" s="77"/>
+      <c r="J16" s="77"/>
+      <c r="K16" s="77"/>
+      <c r="L16" s="77"/>
+      <c r="M16" s="77"/>
+      <c r="N16" s="77"/>
+      <c r="O16" s="77"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A17" s="78"/>
-      <c r="B17" s="78"/>
-      <c r="C17" s="78"/>
-      <c r="D17" s="78"/>
-      <c r="E17" s="78"/>
-      <c r="F17" s="78"/>
-      <c r="G17" s="78"/>
-      <c r="H17" s="78"/>
-      <c r="I17" s="78"/>
-      <c r="J17" s="78"/>
-      <c r="K17" s="78"/>
-      <c r="L17" s="78"/>
-      <c r="M17" s="78"/>
-      <c r="N17" s="78"/>
-      <c r="O17" s="78"/>
+      <c r="A17" s="77"/>
+      <c r="B17" s="77"/>
+      <c r="C17" s="77"/>
+      <c r="D17" s="77"/>
+      <c r="E17" s="77"/>
+      <c r="F17" s="77"/>
+      <c r="G17" s="77"/>
+      <c r="H17" s="77"/>
+      <c r="I17" s="77"/>
+      <c r="J17" s="77"/>
+      <c r="K17" s="77"/>
+      <c r="L17" s="77"/>
+      <c r="M17" s="77"/>
+      <c r="N17" s="77"/>
+      <c r="O17" s="77"/>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A18" s="79"/>
-      <c r="B18" s="79"/>
+      <c r="A18" s="78"/>
+      <c r="B18" s="78"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -13536,272 +13608,272 @@
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B1" s="134"/>
-      <c r="C1" s="134"/>
-      <c r="D1" s="134"/>
-      <c r="E1" s="134"/>
-      <c r="F1" s="134"/>
-      <c r="G1" s="134"/>
-      <c r="H1" s="134"/>
-      <c r="I1" s="134"/>
-      <c r="J1" s="134"/>
-      <c r="K1" s="134"/>
-      <c r="L1" s="134"/>
-      <c r="M1" s="134"/>
-      <c r="N1" s="134"/>
-      <c r="O1" s="134"/>
-      <c r="P1" s="134"/>
-      <c r="Q1" s="134"/>
-      <c r="R1" s="134"/>
-      <c r="S1" s="134"/>
+      <c r="B1" s="133"/>
+      <c r="C1" s="133"/>
+      <c r="D1" s="133"/>
+      <c r="E1" s="133"/>
+      <c r="F1" s="133"/>
+      <c r="G1" s="133"/>
+      <c r="H1" s="133"/>
+      <c r="I1" s="133"/>
+      <c r="J1" s="133"/>
+      <c r="K1" s="133"/>
+      <c r="L1" s="133"/>
+      <c r="M1" s="133"/>
+      <c r="N1" s="133"/>
+      <c r="O1" s="133"/>
+      <c r="P1" s="133"/>
+      <c r="Q1" s="133"/>
+      <c r="R1" s="133"/>
+      <c r="S1" s="133"/>
     </row>
     <row r="2" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B2" s="134"/>
-      <c r="C2" s="134"/>
-      <c r="D2" s="134"/>
-      <c r="E2" s="134"/>
-      <c r="F2" s="134"/>
-      <c r="G2" s="134"/>
-      <c r="H2" s="134"/>
-      <c r="I2" s="134"/>
-      <c r="J2" s="134"/>
-      <c r="K2" s="134"/>
-      <c r="L2" s="134"/>
-      <c r="M2" s="134"/>
-      <c r="N2" s="134"/>
-      <c r="O2" s="134"/>
-      <c r="P2" s="134"/>
-      <c r="Q2" s="134"/>
-      <c r="R2" s="134"/>
-      <c r="S2" s="134"/>
+      <c r="B2" s="133"/>
+      <c r="C2" s="133"/>
+      <c r="D2" s="133"/>
+      <c r="E2" s="133"/>
+      <c r="F2" s="133"/>
+      <c r="G2" s="133"/>
+      <c r="H2" s="133"/>
+      <c r="I2" s="133"/>
+      <c r="J2" s="133"/>
+      <c r="K2" s="133"/>
+      <c r="L2" s="133"/>
+      <c r="M2" s="133"/>
+      <c r="N2" s="133"/>
+      <c r="O2" s="133"/>
+      <c r="P2" s="133"/>
+      <c r="Q2" s="133"/>
+      <c r="R2" s="133"/>
+      <c r="S2" s="133"/>
     </row>
     <row r="3" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B3" s="134"/>
-      <c r="C3" s="134"/>
-      <c r="D3" s="134"/>
-      <c r="E3" s="134"/>
-      <c r="F3" s="134"/>
-      <c r="G3" s="134"/>
-      <c r="H3" s="134"/>
-      <c r="I3" s="134"/>
-      <c r="J3" s="134"/>
-      <c r="K3" s="134"/>
-      <c r="L3" s="134"/>
-      <c r="M3" s="134"/>
-      <c r="N3" s="134"/>
-      <c r="O3" s="134"/>
-      <c r="P3" s="134"/>
-      <c r="Q3" s="134"/>
-      <c r="R3" s="134"/>
-      <c r="S3" s="134"/>
+      <c r="B3" s="133"/>
+      <c r="C3" s="133"/>
+      <c r="D3" s="133"/>
+      <c r="E3" s="133"/>
+      <c r="F3" s="133"/>
+      <c r="G3" s="133"/>
+      <c r="H3" s="133"/>
+      <c r="I3" s="133"/>
+      <c r="J3" s="133"/>
+      <c r="K3" s="133"/>
+      <c r="L3" s="133"/>
+      <c r="M3" s="133"/>
+      <c r="N3" s="133"/>
+      <c r="O3" s="133"/>
+      <c r="P3" s="133"/>
+      <c r="Q3" s="133"/>
+      <c r="R3" s="133"/>
+      <c r="S3" s="133"/>
     </row>
     <row r="4" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B4" s="134"/>
-      <c r="C4" s="135" t="s">
+      <c r="B4" s="133"/>
+      <c r="C4" s="134" t="s">
         <v>40</v>
       </c>
-      <c r="D4" s="135"/>
-      <c r="E4" s="135"/>
-      <c r="F4" s="135"/>
-      <c r="G4" s="135" t="s">
+      <c r="D4" s="134"/>
+      <c r="E4" s="134"/>
+      <c r="F4" s="134"/>
+      <c r="G4" s="134" t="s">
         <v>41</v>
       </c>
-      <c r="H4" s="135"/>
-      <c r="I4" s="135"/>
-      <c r="J4" s="135"/>
-      <c r="K4" s="135" t="s">
+      <c r="H4" s="134"/>
+      <c r="I4" s="134"/>
+      <c r="J4" s="134"/>
+      <c r="K4" s="134" t="s">
         <v>8</v>
       </c>
-      <c r="L4" s="135"/>
-      <c r="M4" s="135"/>
-      <c r="N4" s="135"/>
-      <c r="O4" s="135" t="s">
+      <c r="L4" s="134"/>
+      <c r="M4" s="134"/>
+      <c r="N4" s="134"/>
+      <c r="O4" s="134" t="s">
         <v>42</v>
       </c>
-      <c r="P4" s="135"/>
-      <c r="Q4" s="135"/>
-      <c r="R4" s="135"/>
-      <c r="S4" s="134"/>
+      <c r="P4" s="134"/>
+      <c r="Q4" s="134"/>
+      <c r="R4" s="134"/>
+      <c r="S4" s="133"/>
     </row>
     <row r="5" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B5" s="134"/>
-      <c r="C5" s="135"/>
-      <c r="D5" s="135"/>
-      <c r="E5" s="135"/>
-      <c r="F5" s="135"/>
-      <c r="G5" s="135"/>
-      <c r="H5" s="135"/>
-      <c r="I5" s="135"/>
-      <c r="J5" s="135"/>
-      <c r="K5" s="135"/>
-      <c r="L5" s="135"/>
-      <c r="M5" s="135"/>
-      <c r="N5" s="135"/>
-      <c r="O5" s="135"/>
-      <c r="P5" s="135"/>
-      <c r="Q5" s="135"/>
-      <c r="R5" s="135"/>
-      <c r="S5" s="134"/>
+      <c r="B5" s="133"/>
+      <c r="C5" s="134"/>
+      <c r="D5" s="134"/>
+      <c r="E5" s="134"/>
+      <c r="F5" s="134"/>
+      <c r="G5" s="134"/>
+      <c r="H5" s="134"/>
+      <c r="I5" s="134"/>
+      <c r="J5" s="134"/>
+      <c r="K5" s="134"/>
+      <c r="L5" s="134"/>
+      <c r="M5" s="134"/>
+      <c r="N5" s="134"/>
+      <c r="O5" s="134"/>
+      <c r="P5" s="134"/>
+      <c r="Q5" s="134"/>
+      <c r="R5" s="134"/>
+      <c r="S5" s="133"/>
     </row>
     <row r="6" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B6" s="134"/>
-      <c r="C6" s="135"/>
-      <c r="D6" s="135"/>
-      <c r="E6" s="135"/>
-      <c r="F6" s="135"/>
-      <c r="G6" s="135"/>
-      <c r="H6" s="135"/>
-      <c r="I6" s="135"/>
-      <c r="J6" s="135"/>
-      <c r="K6" s="135"/>
-      <c r="L6" s="135"/>
-      <c r="M6" s="135"/>
-      <c r="N6" s="135"/>
-      <c r="O6" s="135"/>
-      <c r="P6" s="135"/>
-      <c r="Q6" s="135"/>
-      <c r="R6" s="135"/>
-      <c r="S6" s="134"/>
+      <c r="B6" s="133"/>
+      <c r="C6" s="134"/>
+      <c r="D6" s="134"/>
+      <c r="E6" s="134"/>
+      <c r="F6" s="134"/>
+      <c r="G6" s="134"/>
+      <c r="H6" s="134"/>
+      <c r="I6" s="134"/>
+      <c r="J6" s="134"/>
+      <c r="K6" s="134"/>
+      <c r="L6" s="134"/>
+      <c r="M6" s="134"/>
+      <c r="N6" s="134"/>
+      <c r="O6" s="134"/>
+      <c r="P6" s="134"/>
+      <c r="Q6" s="134"/>
+      <c r="R6" s="134"/>
+      <c r="S6" s="133"/>
     </row>
     <row r="7" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B7" s="134"/>
-      <c r="C7" s="134"/>
-      <c r="D7" s="134"/>
-      <c r="E7" s="134"/>
-      <c r="F7" s="134"/>
-      <c r="G7" s="134"/>
-      <c r="H7" s="134"/>
-      <c r="I7" s="134"/>
-      <c r="J7" s="134"/>
-      <c r="K7" s="134"/>
-      <c r="L7" s="134"/>
-      <c r="M7" s="134"/>
-      <c r="N7" s="134"/>
-      <c r="O7" s="134"/>
-      <c r="P7" s="134"/>
-      <c r="Q7" s="134"/>
-      <c r="R7" s="134"/>
-      <c r="S7" s="134"/>
+      <c r="B7" s="133"/>
+      <c r="C7" s="133"/>
+      <c r="D7" s="133"/>
+      <c r="E7" s="133"/>
+      <c r="F7" s="133"/>
+      <c r="G7" s="133"/>
+      <c r="H7" s="133"/>
+      <c r="I7" s="133"/>
+      <c r="J7" s="133"/>
+      <c r="K7" s="133"/>
+      <c r="L7" s="133"/>
+      <c r="M7" s="133"/>
+      <c r="N7" s="133"/>
+      <c r="O7" s="133"/>
+      <c r="P7" s="133"/>
+      <c r="Q7" s="133"/>
+      <c r="R7" s="133"/>
+      <c r="S7" s="133"/>
     </row>
     <row r="8" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B8" s="134"/>
-      <c r="C8" s="134"/>
-      <c r="D8" s="134"/>
-      <c r="E8" s="134"/>
-      <c r="F8" s="134"/>
-      <c r="G8" s="134"/>
-      <c r="H8" s="134"/>
-      <c r="I8" s="134"/>
-      <c r="J8" s="134"/>
-      <c r="K8" s="134"/>
-      <c r="L8" s="134"/>
-      <c r="M8" s="134"/>
-      <c r="N8" s="134"/>
-      <c r="O8" s="134"/>
-      <c r="P8" s="134"/>
-      <c r="Q8" s="134"/>
-      <c r="R8" s="134"/>
-      <c r="S8" s="134"/>
+      <c r="B8" s="133"/>
+      <c r="C8" s="133"/>
+      <c r="D8" s="133"/>
+      <c r="E8" s="133"/>
+      <c r="F8" s="133"/>
+      <c r="G8" s="133"/>
+      <c r="H8" s="133"/>
+      <c r="I8" s="133"/>
+      <c r="J8" s="133"/>
+      <c r="K8" s="133"/>
+      <c r="L8" s="133"/>
+      <c r="M8" s="133"/>
+      <c r="N8" s="133"/>
+      <c r="O8" s="133"/>
+      <c r="P8" s="133"/>
+      <c r="Q8" s="133"/>
+      <c r="R8" s="133"/>
+      <c r="S8" s="133"/>
     </row>
     <row r="9" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B9" s="134"/>
-      <c r="C9" s="134"/>
-      <c r="D9" s="134"/>
-      <c r="E9" s="134"/>
-      <c r="F9" s="134"/>
-      <c r="G9" s="134"/>
-      <c r="H9" s="134"/>
-      <c r="I9" s="134"/>
-      <c r="J9" s="134"/>
-      <c r="K9" s="134"/>
-      <c r="L9" s="134"/>
-      <c r="M9" s="134"/>
-      <c r="N9" s="134"/>
-      <c r="O9" s="134"/>
-      <c r="P9" s="134"/>
-      <c r="Q9" s="134"/>
-      <c r="R9" s="134"/>
-      <c r="S9" s="134"/>
+      <c r="B9" s="133"/>
+      <c r="C9" s="133"/>
+      <c r="D9" s="133"/>
+      <c r="E9" s="133"/>
+      <c r="F9" s="133"/>
+      <c r="G9" s="133"/>
+      <c r="H9" s="133"/>
+      <c r="I9" s="133"/>
+      <c r="J9" s="133"/>
+      <c r="K9" s="133"/>
+      <c r="L9" s="133"/>
+      <c r="M9" s="133"/>
+      <c r="N9" s="133"/>
+      <c r="O9" s="133"/>
+      <c r="P9" s="133"/>
+      <c r="Q9" s="133"/>
+      <c r="R9" s="133"/>
+      <c r="S9" s="133"/>
     </row>
     <row r="10" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B10" s="134"/>
-      <c r="C10" s="134"/>
-      <c r="D10" s="134"/>
-      <c r="E10" s="134"/>
-      <c r="F10" s="134"/>
-      <c r="G10" s="134"/>
-      <c r="H10" s="134"/>
-      <c r="I10" s="134"/>
-      <c r="J10" s="134"/>
-      <c r="K10" s="134"/>
-      <c r="L10" s="134"/>
-      <c r="M10" s="134"/>
-      <c r="N10" s="134"/>
-      <c r="O10" s="134"/>
-      <c r="P10" s="134"/>
-      <c r="Q10" s="134"/>
-      <c r="R10" s="134"/>
-      <c r="S10" s="134"/>
+      <c r="B10" s="133"/>
+      <c r="C10" s="133"/>
+      <c r="D10" s="133"/>
+      <c r="E10" s="133"/>
+      <c r="F10" s="133"/>
+      <c r="G10" s="133"/>
+      <c r="H10" s="133"/>
+      <c r="I10" s="133"/>
+      <c r="J10" s="133"/>
+      <c r="K10" s="133"/>
+      <c r="L10" s="133"/>
+      <c r="M10" s="133"/>
+      <c r="N10" s="133"/>
+      <c r="O10" s="133"/>
+      <c r="P10" s="133"/>
+      <c r="Q10" s="133"/>
+      <c r="R10" s="133"/>
+      <c r="S10" s="133"/>
     </row>
     <row r="11" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B11" s="134"/>
-      <c r="C11" s="134"/>
-      <c r="D11" s="134"/>
-      <c r="E11" s="134"/>
-      <c r="F11" s="134"/>
-      <c r="G11" s="134"/>
-      <c r="H11" s="134"/>
-      <c r="I11" s="134"/>
-      <c r="J11" s="134"/>
-      <c r="K11" s="134"/>
-      <c r="L11" s="134"/>
-      <c r="M11" s="134"/>
-      <c r="N11" s="134"/>
-      <c r="O11" s="134"/>
-      <c r="P11" s="134"/>
-      <c r="Q11" s="134"/>
-      <c r="R11" s="134"/>
-      <c r="S11" s="134"/>
+      <c r="B11" s="133"/>
+      <c r="C11" s="133"/>
+      <c r="D11" s="133"/>
+      <c r="E11" s="133"/>
+      <c r="F11" s="133"/>
+      <c r="G11" s="133"/>
+      <c r="H11" s="133"/>
+      <c r="I11" s="133"/>
+      <c r="J11" s="133"/>
+      <c r="K11" s="133"/>
+      <c r="L11" s="133"/>
+      <c r="M11" s="133"/>
+      <c r="N11" s="133"/>
+      <c r="O11" s="133"/>
+      <c r="P11" s="133"/>
+      <c r="Q11" s="133"/>
+      <c r="R11" s="133"/>
+      <c r="S11" s="133"/>
     </row>
     <row r="12" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B12" s="134"/>
-      <c r="C12" s="134"/>
-      <c r="D12" s="134"/>
-      <c r="E12" s="134"/>
-      <c r="F12" s="134"/>
-      <c r="G12" s="134"/>
-      <c r="H12" s="134"/>
-      <c r="I12" s="134"/>
-      <c r="J12" s="134"/>
-      <c r="K12" s="134"/>
-      <c r="L12" s="134"/>
-      <c r="M12" s="134"/>
-      <c r="N12" s="134"/>
-      <c r="O12" s="134"/>
-      <c r="P12" s="134"/>
-      <c r="Q12" s="134"/>
-      <c r="R12" s="134"/>
-      <c r="S12" s="134"/>
+      <c r="B12" s="133"/>
+      <c r="C12" s="133"/>
+      <c r="D12" s="133"/>
+      <c r="E12" s="133"/>
+      <c r="F12" s="133"/>
+      <c r="G12" s="133"/>
+      <c r="H12" s="133"/>
+      <c r="I12" s="133"/>
+      <c r="J12" s="133"/>
+      <c r="K12" s="133"/>
+      <c r="L12" s="133"/>
+      <c r="M12" s="133"/>
+      <c r="N12" s="133"/>
+      <c r="O12" s="133"/>
+      <c r="P12" s="133"/>
+      <c r="Q12" s="133"/>
+      <c r="R12" s="133"/>
+      <c r="S12" s="133"/>
     </row>
     <row r="13" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B13" s="134"/>
-      <c r="C13" s="134"/>
-      <c r="D13" s="134"/>
-      <c r="E13" s="134"/>
-      <c r="F13" s="134"/>
-      <c r="G13" s="134"/>
-      <c r="H13" s="134"/>
-      <c r="I13" s="134"/>
-      <c r="J13" s="134"/>
-      <c r="K13" s="134"/>
-      <c r="L13" s="134"/>
-      <c r="M13" s="134"/>
-      <c r="N13" s="134"/>
-      <c r="O13" s="134"/>
-      <c r="P13" s="134"/>
-      <c r="Q13" s="134"/>
-      <c r="R13" s="134"/>
-      <c r="S13" s="134"/>
+      <c r="B13" s="133"/>
+      <c r="C13" s="133"/>
+      <c r="D13" s="133"/>
+      <c r="E13" s="133"/>
+      <c r="F13" s="133"/>
+      <c r="G13" s="133"/>
+      <c r="H13" s="133"/>
+      <c r="I13" s="133"/>
+      <c r="J13" s="133"/>
+      <c r="K13" s="133"/>
+      <c r="L13" s="133"/>
+      <c r="M13" s="133"/>
+      <c r="N13" s="133"/>
+      <c r="O13" s="133"/>
+      <c r="P13" s="133"/>
+      <c r="Q13" s="133"/>
+      <c r="R13" s="133"/>
+      <c r="S13" s="133"/>
     </row>
   </sheetData>
   <mergeCells count="8">

</xml_diff>